<commit_message>
I changed source file
</commit_message>
<xml_diff>
--- a/source_file/jquery_testscenario.xlsx
+++ b/source_file/jquery_testscenario.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gturd\IdeaProjects\FirstAssignment\source_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4BBDF0-43CC-47E9-99DF-E0C39C260218}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD56A360-00F1-4469-B3CC-B4CF482C4B25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{CE714CED-6ED2-47BF-9249-83F3ACACC2F2}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="332">
   <si>
     <t>Project Name:</t>
   </si>
@@ -371,18 +371,6 @@
   </si>
   <si>
     <t>The Selectable page is displayed</t>
-  </si>
-  <si>
-    <t>Use the cursor to select item</t>
-  </si>
-  <si>
-    <t>The item should be selected</t>
-  </si>
-  <si>
-    <t>The item is slected</t>
-  </si>
-  <si>
-    <t>Verify the item is selected</t>
   </si>
   <si>
     <t>Use the cursor to select multiple items</t>
@@ -1609,6 +1597,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1622,12 +1616,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2177,10 +2165,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E61229-28C4-4005-AC6C-FBD77E5B6143}">
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,7 +2184,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2217,7 +2205,7 @@
       <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="60"/>
+      <c r="A2" s="62"/>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
@@ -2278,26 +2266,26 @@
       <c r="A6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
       <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2390,10 +2378,10 @@
       </c>
       <c r="F12" s="32"/>
       <c r="G12" s="45" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="H12" s="45" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="I12" s="33"/>
     </row>
@@ -2485,10 +2473,10 @@
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="45" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="H17" s="45" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="I17" s="33"/>
     </row>
@@ -2692,10 +2680,10 @@
       </c>
       <c r="F28" s="32"/>
       <c r="G28" s="45" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="H28" s="45" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="I28" s="33"/>
     </row>
@@ -2716,7 +2704,7 @@
       </c>
       <c r="I29" s="33"/>
     </row>
-    <row r="30" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A30" s="30"/>
       <c r="B30" s="31"/>
       <c r="C30" s="32"/>
@@ -2729,7 +2717,7 @@
         <v>116</v>
       </c>
       <c r="H30" s="45" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I30" s="33"/>
     </row>
@@ -2738,15 +2726,15 @@
       <c r="B31" s="31"/>
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
-      <c r="E31" s="54" t="s">
-        <v>118</v>
+      <c r="E31" s="53" t="s">
+        <v>117</v>
       </c>
       <c r="F31" s="32"/>
       <c r="G31" s="45" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H31" s="45" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="I31" s="33"/>
     </row>
@@ -2756,92 +2744,92 @@
       <c r="C32" s="32"/>
       <c r="D32" s="32"/>
       <c r="E32" s="45" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F32" s="32"/>
       <c r="G32" s="45" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H32" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="I32" s="33"/>
+    </row>
+    <row r="33" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="I32" s="33"/>
-    </row>
-    <row r="33" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="53" t="s">
-        <v>121</v>
-      </c>
-      <c r="F33" s="32"/>
+      <c r="C33" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G33" s="45" t="s">
-        <v>122</v>
+        <v>64</v>
       </c>
       <c r="H33" s="45" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="I33" s="33"/>
     </row>
-    <row r="34" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A34" s="30"/>
       <c r="B34" s="31"/>
       <c r="C34" s="32"/>
       <c r="D34" s="32"/>
-      <c r="E34" s="45" t="s">
-        <v>125</v>
+      <c r="E34" s="32" t="s">
+        <v>127</v>
       </c>
       <c r="F34" s="32"/>
       <c r="G34" s="45" t="s">
-        <v>126</v>
+        <v>327</v>
       </c>
       <c r="H34" s="45" t="s">
+        <v>328</v>
+      </c>
+      <c r="I34" s="33"/>
+    </row>
+    <row r="35" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="30"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="F35" s="32"/>
+      <c r="G35" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="I34" s="33"/>
-    </row>
-    <row r="35" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="51" t="s">
-        <v>127</v>
-      </c>
-      <c r="C35" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="D35" s="45" t="s">
+      <c r="H35" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="E35" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="F35" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="G35" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="H35" s="45" t="s">
-        <v>74</v>
-      </c>
       <c r="I35" s="33"/>
     </row>
-    <row r="36" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A36" s="30"/>
       <c r="B36" s="31"/>
       <c r="C36" s="32"/>
       <c r="D36" s="32"/>
-      <c r="E36" s="32" t="s">
+      <c r="E36" s="45" t="s">
         <v>131</v>
       </c>
       <c r="F36" s="32"/>
       <c r="G36" s="45" t="s">
-        <v>331</v>
+        <v>132</v>
       </c>
       <c r="H36" s="45" t="s">
-        <v>332</v>
+        <v>133</v>
       </c>
       <c r="I36" s="33"/>
     </row>
@@ -2851,122 +2839,122 @@
       <c r="C37" s="32"/>
       <c r="D37" s="32"/>
       <c r="E37" s="54" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F37" s="32"/>
       <c r="G37" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="H37" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="H37" s="45" t="s">
-        <v>134</v>
-      </c>
       <c r="I37" s="33"/>
     </row>
-    <row r="38" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="45" t="s">
+    <row r="38" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="51" t="s">
         <v>135</v>
       </c>
-      <c r="F38" s="32"/>
+      <c r="C38" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G38" s="45" t="s">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="H38" s="45" t="s">
-        <v>137</v>
+        <v>74</v>
       </c>
       <c r="I38" s="33"/>
     </row>
-    <row r="39" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A39" s="30"/>
       <c r="B39" s="31"/>
       <c r="C39" s="32"/>
       <c r="D39" s="32"/>
-      <c r="E39" s="54" t="s">
-        <v>138</v>
+      <c r="E39" s="32" t="s">
+        <v>139</v>
       </c>
       <c r="F39" s="32"/>
       <c r="G39" s="45" t="s">
-        <v>136</v>
+        <v>329</v>
       </c>
       <c r="H39" s="45" t="s">
-        <v>137</v>
+        <v>330</v>
       </c>
       <c r="I39" s="33"/>
     </row>
-    <row r="40" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="49" t="s">
+    <row r="40" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="30"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="F40" s="32"/>
+      <c r="G40" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="B40" s="51" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" s="53" t="s">
-        <v>140</v>
-      </c>
-      <c r="D40" s="45" t="s">
+      <c r="H40" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="E40" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="F40" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="G40" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="H40" s="45" t="s">
-        <v>74</v>
-      </c>
       <c r="I40" s="33"/>
     </row>
-    <row r="41" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A41" s="30"/>
       <c r="B41" s="31"/>
       <c r="C41" s="32"/>
       <c r="D41" s="32"/>
-      <c r="E41" s="32" t="s">
+      <c r="E41" s="45" t="s">
         <v>143</v>
       </c>
       <c r="F41" s="32"/>
-      <c r="G41" s="45" t="s">
-        <v>333</v>
+      <c r="G41" s="55" t="s">
+        <v>144</v>
       </c>
       <c r="H41" s="45" t="s">
-        <v>334</v>
+        <v>145</v>
       </c>
       <c r="I41" s="33"/>
     </row>
-    <row r="42" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A42" s="30"/>
       <c r="B42" s="31"/>
       <c r="C42" s="32"/>
       <c r="D42" s="32"/>
       <c r="E42" s="54" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F42" s="32"/>
       <c r="G42" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="H42" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="H42" s="45" t="s">
-        <v>146</v>
-      </c>
       <c r="I42" s="33"/>
     </row>
-    <row r="43" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A43" s="30"/>
       <c r="B43" s="31"/>
       <c r="C43" s="32"/>
       <c r="D43" s="32"/>
-      <c r="E43" s="45" t="s">
+      <c r="E43" s="32" t="s">
         <v>147</v>
       </c>
       <c r="F43" s="32"/>
-      <c r="G43" s="55" t="s">
+      <c r="G43" s="45" t="s">
         <v>148</v>
       </c>
       <c r="H43" s="45" t="s">
@@ -2974,91 +2962,91 @@
       </c>
       <c r="I43" s="33"/>
     </row>
-    <row r="44" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="54" t="s">
+    <row r="44" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="51" t="s">
         <v>150</v>
       </c>
-      <c r="F44" s="32"/>
+      <c r="C44" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="D44" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="E44" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F44" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G44" s="45" t="s">
-        <v>148</v>
+        <v>64</v>
       </c>
       <c r="H44" s="45" t="s">
-        <v>149</v>
+        <v>74</v>
       </c>
       <c r="I44" s="33"/>
     </row>
-    <row r="45" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
       <c r="B45" s="31"/>
       <c r="C45" s="32"/>
       <c r="D45" s="32"/>
-      <c r="E45" s="32" t="s">
-        <v>151</v>
+      <c r="E45" s="45" t="s">
+        <v>153</v>
       </c>
       <c r="F45" s="32"/>
       <c r="G45" s="45" t="s">
-        <v>152</v>
+        <v>331</v>
       </c>
       <c r="H45" s="45" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I45" s="33"/>
     </row>
-    <row r="46" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="B46" s="51" t="s">
-        <v>154</v>
-      </c>
-      <c r="C46" s="53" t="s">
+    <row r="46" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="A46" s="30"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="54" t="s">
         <v>155</v>
       </c>
-      <c r="D46" s="45" t="s">
+      <c r="F46" s="32"/>
+      <c r="G46" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="E46" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="F46" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="G46" s="45" t="s">
-        <v>64</v>
-      </c>
       <c r="H46" s="45" t="s">
-        <v>74</v>
+        <v>157</v>
       </c>
       <c r="I46" s="33"/>
     </row>
-    <row r="47" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A47" s="30"/>
       <c r="B47" s="31"/>
       <c r="C47" s="32"/>
       <c r="D47" s="32"/>
       <c r="E47" s="45" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F47" s="32"/>
       <c r="G47" s="45" t="s">
-        <v>335</v>
+        <v>159</v>
       </c>
       <c r="H47" s="45" t="s">
         <v>158</v>
       </c>
       <c r="I47" s="33"/>
     </row>
-    <row r="48" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A48" s="30"/>
       <c r="B48" s="31"/>
       <c r="C48" s="32"/>
       <c r="D48" s="32"/>
       <c r="E48" s="54" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F48" s="32"/>
       <c r="G48" s="45" t="s">
@@ -3070,78 +3058,78 @@
       <c r="I48" s="33"/>
     </row>
     <row r="49" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
-      <c r="B49" s="31"/>
+      <c r="A49" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="51" t="s">
+        <v>178</v>
+      </c>
       <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="45" t="s">
-        <v>162</v>
-      </c>
-      <c r="F49" s="32"/>
+      <c r="D49" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="E49" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F49" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G49" s="45" t="s">
-        <v>163</v>
+        <v>64</v>
       </c>
       <c r="H49" s="45" t="s">
-        <v>162</v>
+        <v>74</v>
       </c>
       <c r="I49" s="33"/>
     </row>
-    <row r="50" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A50" s="30"/>
       <c r="B50" s="31"/>
       <c r="C50" s="32"/>
       <c r="D50" s="32"/>
-      <c r="E50" s="54" t="s">
-        <v>166</v>
+      <c r="E50" s="32" t="s">
+        <v>164</v>
       </c>
       <c r="F50" s="32"/>
       <c r="G50" s="45" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H50" s="45" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I50" s="33"/>
     </row>
-    <row r="51" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" s="51" t="s">
-        <v>182</v>
-      </c>
+    <row r="51" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="30"/>
+      <c r="B51" s="31"/>
       <c r="C51" s="32"/>
-      <c r="D51" s="45" t="s">
+      <c r="D51" s="32"/>
+      <c r="E51" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="E51" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="F51" s="47" t="s">
-        <v>63</v>
-      </c>
+      <c r="F51" s="32"/>
       <c r="G51" s="45" t="s">
-        <v>64</v>
+        <v>168</v>
       </c>
       <c r="H51" s="45" t="s">
-        <v>74</v>
+        <v>169</v>
       </c>
       <c r="I51" s="33"/>
     </row>
-    <row r="52" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A52" s="30"/>
       <c r="B52" s="31"/>
       <c r="C52" s="32"/>
       <c r="D52" s="32"/>
-      <c r="E52" s="32" t="s">
-        <v>168</v>
+      <c r="E52" s="45" t="s">
+        <v>170</v>
       </c>
       <c r="F52" s="32"/>
       <c r="G52" s="45" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H52" s="45" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="I52" s="33"/>
     </row>
@@ -3151,14 +3139,14 @@
       <c r="C53" s="32"/>
       <c r="D53" s="32"/>
       <c r="E53" s="54" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F53" s="32"/>
       <c r="G53" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="H53" s="45" t="s">
         <v>172</v>
-      </c>
-      <c r="H53" s="45" t="s">
-        <v>173</v>
       </c>
       <c r="I53" s="33"/>
     </row>
@@ -3180,7 +3168,7 @@
       <c r="I54" s="33"/>
     </row>
     <row r="55" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
+      <c r="A55" s="51"/>
       <c r="B55" s="31"/>
       <c r="C55" s="32"/>
       <c r="D55" s="32"/>
@@ -3196,206 +3184,206 @@
       </c>
       <c r="I55" s="33"/>
     </row>
-    <row r="56" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A56" s="30"/>
-      <c r="B56" s="31"/>
+    <row r="56" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B56" s="51" t="s">
+        <v>179</v>
+      </c>
       <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="45" t="s">
-        <v>178</v>
-      </c>
-      <c r="F56" s="32"/>
+      <c r="D56" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="E56" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F56" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G56" s="45" t="s">
-        <v>179</v>
+        <v>64</v>
       </c>
       <c r="H56" s="45" t="s">
-        <v>180</v>
+        <v>74</v>
       </c>
       <c r="I56" s="33"/>
     </row>
-    <row r="57" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A57" s="51"/>
+    <row r="57" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="30"/>
       <c r="B57" s="31"/>
       <c r="C57" s="32"/>
       <c r="D57" s="32"/>
-      <c r="E57" s="54" t="s">
-        <v>181</v>
+      <c r="E57" s="45" t="s">
+        <v>180</v>
       </c>
       <c r="F57" s="32"/>
       <c r="G57" s="45" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H57" s="45" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I57" s="33"/>
     </row>
-    <row r="58" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="B58" s="51" t="s">
+    <row r="58" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A58" s="30"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="C58" s="32"/>
-      <c r="D58" s="45" t="s">
-        <v>167</v>
-      </c>
-      <c r="E58" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="F58" s="47" t="s">
-        <v>63</v>
-      </c>
+      <c r="F58" s="32"/>
       <c r="G58" s="45" t="s">
-        <v>64</v>
+        <v>184</v>
       </c>
       <c r="H58" s="45" t="s">
-        <v>74</v>
+        <v>185</v>
       </c>
       <c r="I58" s="33"/>
     </row>
-    <row r="59" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A59" s="30"/>
       <c r="B59" s="31"/>
       <c r="C59" s="32"/>
       <c r="D59" s="32"/>
       <c r="E59" s="45" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="F59" s="32"/>
-      <c r="G59" s="45" t="s">
-        <v>185</v>
+      <c r="G59" s="56" t="s">
+        <v>186</v>
       </c>
       <c r="H59" s="45" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I59" s="33"/>
     </row>
-    <row r="60" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A60" s="30"/>
       <c r="B60" s="31"/>
       <c r="C60" s="32"/>
       <c r="D60" s="32"/>
       <c r="E60" s="54" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F60" s="32"/>
       <c r="G60" s="45" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H60" s="45" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I60" s="33"/>
     </row>
-    <row r="61" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A61" s="30"/>
       <c r="B61" s="31"/>
       <c r="C61" s="32"/>
       <c r="D61" s="32"/>
       <c r="E61" s="45" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F61" s="32"/>
-      <c r="G61" s="56" t="s">
-        <v>190</v>
+      <c r="G61" s="45" t="s">
+        <v>191</v>
       </c>
       <c r="H61" s="45" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I61" s="33"/>
     </row>
-    <row r="62" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="30"/>
       <c r="B62" s="31"/>
       <c r="C62" s="32"/>
       <c r="D62" s="32"/>
-      <c r="E62" s="54" t="s">
-        <v>192</v>
+      <c r="E62" s="53" t="s">
+        <v>193</v>
       </c>
       <c r="F62" s="32"/>
       <c r="G62" s="45" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H62" s="45" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I62" s="33"/>
     </row>
-    <row r="63" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
-      <c r="B63" s="31"/>
+    <row r="63" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" s="57" t="s">
+        <v>194</v>
+      </c>
       <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="45" t="s">
-        <v>194</v>
-      </c>
-      <c r="F63" s="32"/>
+      <c r="D63" s="45" t="s">
+        <v>207</v>
+      </c>
+      <c r="E63" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F63" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G63" s="45" t="s">
-        <v>195</v>
+        <v>64</v>
       </c>
       <c r="H63" s="45" t="s">
-        <v>196</v>
+        <v>74</v>
       </c>
       <c r="I63" s="33"/>
     </row>
-    <row r="64" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A64" s="30"/>
       <c r="B64" s="31"/>
       <c r="C64" s="32"/>
       <c r="D64" s="32"/>
-      <c r="E64" s="53" t="s">
-        <v>197</v>
+      <c r="E64" s="45" t="s">
+        <v>195</v>
       </c>
       <c r="F64" s="32"/>
       <c r="G64" s="45" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H64" s="45" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I64" s="33"/>
     </row>
-    <row r="65" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="B65" s="57" t="s">
+    <row r="65" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A65" s="30"/>
+      <c r="B65" s="31"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="54" t="s">
         <v>198</v>
       </c>
-      <c r="C65" s="32"/>
-      <c r="D65" s="45" t="s">
-        <v>211</v>
-      </c>
-      <c r="E65" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="F65" s="47" t="s">
-        <v>63</v>
-      </c>
+      <c r="F65" s="32"/>
       <c r="G65" s="45" t="s">
-        <v>64</v>
+        <v>199</v>
       </c>
       <c r="H65" s="45" t="s">
-        <v>74</v>
+        <v>200</v>
       </c>
       <c r="I65" s="33"/>
     </row>
-    <row r="66" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A66" s="30"/>
       <c r="B66" s="31"/>
       <c r="C66" s="32"/>
       <c r="D66" s="32"/>
       <c r="E66" s="45" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F66" s="32"/>
       <c r="G66" s="45" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="H66" s="45" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="I66" s="33"/>
     </row>
@@ -3405,124 +3393,124 @@
       <c r="C67" s="32"/>
       <c r="D67" s="32"/>
       <c r="E67" s="54" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F67" s="32"/>
       <c r="G67" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="H67" s="45" t="s">
         <v>203</v>
       </c>
-      <c r="H67" s="45" t="s">
-        <v>204</v>
-      </c>
       <c r="I67" s="33"/>
     </row>
-    <row r="68" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A68" s="30"/>
-      <c r="B68" s="31"/>
+    <row r="68" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68" s="51" t="s">
+        <v>206</v>
+      </c>
       <c r="C68" s="32"/>
-      <c r="D68" s="32"/>
-      <c r="E68" s="45" t="s">
-        <v>205</v>
-      </c>
-      <c r="F68" s="32"/>
+      <c r="D68" s="45" t="s">
+        <v>225</v>
+      </c>
+      <c r="E68" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F68" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G68" s="45" t="s">
-        <v>206</v>
+        <v>64</v>
       </c>
       <c r="H68" s="45" t="s">
-        <v>207</v>
+        <v>74</v>
       </c>
       <c r="I68" s="33"/>
     </row>
-    <row r="69" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A69" s="30"/>
       <c r="B69" s="31"/>
       <c r="C69" s="32"/>
       <c r="D69" s="32"/>
-      <c r="E69" s="54" t="s">
+      <c r="E69" s="32" t="s">
         <v>208</v>
       </c>
       <c r="F69" s="32"/>
       <c r="G69" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="H69" s="45" t="s">
         <v>209</v>
       </c>
-      <c r="H69" s="45" t="s">
-        <v>207</v>
-      </c>
       <c r="I69" s="33"/>
     </row>
-    <row r="70" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="B70" s="51" t="s">
-        <v>210</v>
-      </c>
+    <row r="70" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A70" s="30"/>
+      <c r="B70" s="31"/>
       <c r="C70" s="32"/>
-      <c r="D70" s="45" t="s">
-        <v>229</v>
-      </c>
-      <c r="E70" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="F70" s="47" t="s">
-        <v>63</v>
-      </c>
+      <c r="D70" s="32"/>
+      <c r="E70" s="54" t="s">
+        <v>211</v>
+      </c>
+      <c r="F70" s="32"/>
       <c r="G70" s="45" t="s">
-        <v>64</v>
+        <v>212</v>
       </c>
       <c r="H70" s="45" t="s">
-        <v>74</v>
+        <v>213</v>
       </c>
       <c r="I70" s="33"/>
     </row>
-    <row r="71" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A71" s="30"/>
       <c r="B71" s="31"/>
       <c r="C71" s="32"/>
       <c r="D71" s="32"/>
-      <c r="E71" s="32" t="s">
-        <v>212</v>
+      <c r="E71" s="45" t="s">
+        <v>214</v>
       </c>
       <c r="F71" s="32"/>
       <c r="G71" s="45" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H71" s="45" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="I71" s="33"/>
     </row>
-    <row r="72" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A72" s="30"/>
       <c r="B72" s="31"/>
       <c r="C72" s="32"/>
       <c r="D72" s="32"/>
-      <c r="E72" s="54" t="s">
-        <v>215</v>
+      <c r="E72" s="45" t="s">
+        <v>217</v>
       </c>
       <c r="F72" s="32"/>
       <c r="G72" s="45" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="H72" s="45" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="I72" s="33"/>
     </row>
-    <row r="73" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A73" s="30"/>
       <c r="B73" s="31"/>
       <c r="C73" s="32"/>
       <c r="D73" s="32"/>
       <c r="E73" s="45" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F73" s="32"/>
       <c r="G73" s="45" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H73" s="45" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="I73" s="33"/>
     </row>
@@ -3531,184 +3519,184 @@
       <c r="B74" s="31"/>
       <c r="C74" s="32"/>
       <c r="D74" s="32"/>
-      <c r="E74" s="45" t="s">
-        <v>221</v>
+      <c r="E74" s="54" t="s">
+        <v>223</v>
       </c>
       <c r="F74" s="32"/>
       <c r="G74" s="45" t="s">
+        <v>221</v>
+      </c>
+      <c r="H74" s="45" t="s">
         <v>222</v>
       </c>
-      <c r="H74" s="45" t="s">
-        <v>223</v>
-      </c>
       <c r="I74" s="33"/>
     </row>
-    <row r="75" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="30"/>
-      <c r="B75" s="31"/>
+    <row r="75" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" s="51" t="s">
+        <v>224</v>
+      </c>
       <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
+      <c r="D75" s="45" t="s">
+        <v>226</v>
+      </c>
       <c r="E75" s="45" t="s">
-        <v>224</v>
-      </c>
-      <c r="F75" s="32"/>
+        <v>62</v>
+      </c>
+      <c r="F75" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G75" s="45" t="s">
-        <v>225</v>
+        <v>64</v>
       </c>
       <c r="H75" s="45" t="s">
-        <v>226</v>
+        <v>74</v>
       </c>
       <c r="I75" s="33"/>
     </row>
-    <row r="76" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A76" s="30"/>
       <c r="B76" s="31"/>
       <c r="C76" s="32"/>
       <c r="D76" s="32"/>
-      <c r="E76" s="54" t="s">
+      <c r="E76" s="45" t="s">
         <v>227</v>
       </c>
       <c r="F76" s="32"/>
       <c r="G76" s="45" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="H76" s="45" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="I76" s="33"/>
     </row>
-    <row r="77" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="B77" s="51" t="s">
-        <v>228</v>
-      </c>
+    <row r="77" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A77" s="30"/>
+      <c r="B77" s="31"/>
       <c r="C77" s="32"/>
-      <c r="D77" s="45" t="s">
+      <c r="D77" s="32"/>
+      <c r="E77" s="54" t="s">
         <v>230</v>
       </c>
-      <c r="E77" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="F77" s="47" t="s">
-        <v>63</v>
-      </c>
+      <c r="F77" s="32"/>
       <c r="G77" s="45" t="s">
-        <v>64</v>
+        <v>231</v>
       </c>
       <c r="H77" s="45" t="s">
-        <v>74</v>
+        <v>232</v>
       </c>
       <c r="I77" s="33"/>
     </row>
-    <row r="78" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A78" s="30"/>
       <c r="B78" s="31"/>
       <c r="C78" s="32"/>
       <c r="D78" s="32"/>
       <c r="E78" s="45" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F78" s="32"/>
       <c r="G78" s="45" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H78" s="45" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I78" s="33"/>
     </row>
-    <row r="79" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A79" s="30"/>
       <c r="B79" s="31"/>
       <c r="C79" s="32"/>
       <c r="D79" s="32"/>
-      <c r="E79" s="54" t="s">
-        <v>234</v>
+      <c r="E79" s="45" t="s">
+        <v>236</v>
       </c>
       <c r="F79" s="32"/>
       <c r="G79" s="45" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="H79" s="45" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="I79" s="33"/>
     </row>
-    <row r="80" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="30"/>
-      <c r="B80" s="31"/>
+    <row r="80" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B80" s="51" t="s">
+        <v>239</v>
+      </c>
       <c r="C80" s="32"/>
-      <c r="D80" s="32"/>
+      <c r="D80" s="45" t="s">
+        <v>240</v>
+      </c>
       <c r="E80" s="45" t="s">
-        <v>238</v>
-      </c>
-      <c r="F80" s="32"/>
+        <v>62</v>
+      </c>
+      <c r="F80" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G80" s="45" t="s">
-        <v>237</v>
+        <v>64</v>
       </c>
       <c r="H80" s="45" t="s">
-        <v>239</v>
+        <v>74</v>
       </c>
       <c r="I80" s="33"/>
     </row>
-    <row r="81" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A81" s="30"/>
       <c r="B81" s="31"/>
       <c r="C81" s="32"/>
       <c r="D81" s="32"/>
       <c r="E81" s="45" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F81" s="32"/>
       <c r="G81" s="45" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H81" s="45" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I81" s="33"/>
     </row>
-    <row r="82" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="58" t="s">
-        <v>34</v>
-      </c>
-      <c r="B82" s="51" t="s">
-        <v>243</v>
-      </c>
+    <row r="82" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A82" s="30"/>
+      <c r="B82" s="31"/>
       <c r="C82" s="32"/>
-      <c r="D82" s="45" t="s">
+      <c r="D82" s="32"/>
+      <c r="E82" s="54" t="s">
         <v>244</v>
       </c>
-      <c r="E82" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="F82" s="47" t="s">
-        <v>63</v>
-      </c>
+      <c r="F82" s="32"/>
       <c r="G82" s="45" t="s">
-        <v>64</v>
+        <v>245</v>
       </c>
       <c r="H82" s="45" t="s">
-        <v>74</v>
+        <v>246</v>
       </c>
       <c r="I82" s="33"/>
     </row>
-    <row r="83" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A83" s="30"/>
       <c r="B83" s="31"/>
       <c r="C83" s="32"/>
       <c r="D83" s="32"/>
       <c r="E83" s="45" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F83" s="32"/>
       <c r="G83" s="45" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="H83" s="45" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="I83" s="33"/>
     </row>
@@ -3718,107 +3706,107 @@
       <c r="C84" s="32"/>
       <c r="D84" s="32"/>
       <c r="E84" s="54" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F84" s="32"/>
       <c r="G84" s="45" t="s">
+        <v>248</v>
+      </c>
+      <c r="H84" s="45" t="s">
         <v>249</v>
       </c>
-      <c r="H84" s="45" t="s">
-        <v>250</v>
-      </c>
       <c r="I84" s="33"/>
     </row>
-    <row r="85" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A85" s="30"/>
-      <c r="B85" s="31"/>
+    <row r="85" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B85" s="51" t="s">
+        <v>251</v>
+      </c>
       <c r="C85" s="32"/>
-      <c r="D85" s="32"/>
-      <c r="E85" s="45" t="s">
-        <v>251</v>
-      </c>
-      <c r="F85" s="32"/>
+      <c r="D85" s="45" t="s">
+        <v>252</v>
+      </c>
+      <c r="E85" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F85" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G85" s="45" t="s">
-        <v>252</v>
+        <v>64</v>
       </c>
       <c r="H85" s="45" t="s">
-        <v>253</v>
+        <v>74</v>
       </c>
       <c r="I85" s="33"/>
     </row>
-    <row r="86" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A86" s="30"/>
       <c r="B86" s="31"/>
       <c r="C86" s="32"/>
       <c r="D86" s="32"/>
-      <c r="E86" s="54" t="s">
-        <v>254</v>
+      <c r="E86" s="32" t="s">
+        <v>253</v>
       </c>
       <c r="F86" s="32"/>
       <c r="G86" s="45" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="H86" s="45" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="I86" s="33"/>
     </row>
-    <row r="87" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="58" t="s">
-        <v>36</v>
-      </c>
-      <c r="B87" s="51" t="s">
-        <v>255</v>
-      </c>
+    <row r="87" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A87" s="30"/>
+      <c r="B87" s="31"/>
       <c r="C87" s="32"/>
-      <c r="D87" s="45" t="s">
+      <c r="D87" s="32"/>
+      <c r="E87" s="54" t="s">
         <v>256</v>
       </c>
-      <c r="E87" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="F87" s="47" t="s">
-        <v>63</v>
-      </c>
+      <c r="F87" s="32"/>
       <c r="G87" s="45" t="s">
-        <v>64</v>
+        <v>257</v>
       </c>
       <c r="H87" s="45" t="s">
-        <v>74</v>
+        <v>258</v>
       </c>
       <c r="I87" s="33"/>
     </row>
-    <row r="88" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A88" s="30"/>
       <c r="B88" s="31"/>
       <c r="C88" s="32"/>
       <c r="D88" s="32"/>
-      <c r="E88" s="32" t="s">
-        <v>257</v>
+      <c r="E88" s="45" t="s">
+        <v>259</v>
       </c>
       <c r="F88" s="32"/>
       <c r="G88" s="45" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="H88" s="45" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="I88" s="33"/>
     </row>
-    <row r="89" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A89" s="30"/>
       <c r="B89" s="31"/>
       <c r="C89" s="32"/>
       <c r="D89" s="32"/>
-      <c r="E89" s="54" t="s">
-        <v>260</v>
+      <c r="E89" s="45" t="s">
+        <v>271</v>
       </c>
       <c r="F89" s="32"/>
       <c r="G89" s="45" t="s">
+        <v>260</v>
+      </c>
+      <c r="H89" s="45" t="s">
         <v>261</v>
-      </c>
-      <c r="H89" s="45" t="s">
-        <v>262</v>
       </c>
       <c r="I89" s="33"/>
     </row>
@@ -3828,14 +3816,14 @@
       <c r="C90" s="32"/>
       <c r="D90" s="32"/>
       <c r="E90" s="45" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F90" s="32"/>
       <c r="G90" s="45" t="s">
+        <v>263</v>
+      </c>
+      <c r="H90" s="45" t="s">
         <v>264</v>
-      </c>
-      <c r="H90" s="45" t="s">
-        <v>265</v>
       </c>
       <c r="I90" s="33"/>
     </row>
@@ -3845,14 +3833,14 @@
       <c r="C91" s="32"/>
       <c r="D91" s="32"/>
       <c r="E91" s="45" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F91" s="32"/>
       <c r="G91" s="45" t="s">
+        <v>263</v>
+      </c>
+      <c r="H91" s="45" t="s">
         <v>264</v>
-      </c>
-      <c r="H91" s="45" t="s">
-        <v>265</v>
       </c>
       <c r="I91" s="33"/>
     </row>
@@ -3862,14 +3850,14 @@
       <c r="C92" s="32"/>
       <c r="D92" s="32"/>
       <c r="E92" s="45" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F92" s="32"/>
       <c r="G92" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="H92" s="45" t="s">
         <v>267</v>
-      </c>
-      <c r="H92" s="45" t="s">
-        <v>268</v>
       </c>
       <c r="I92" s="33"/>
     </row>
@@ -3879,14 +3867,14 @@
       <c r="C93" s="32"/>
       <c r="D93" s="32"/>
       <c r="E93" s="45" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F93" s="32"/>
       <c r="G93" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="H93" s="45" t="s">
         <v>267</v>
-      </c>
-      <c r="H93" s="45" t="s">
-        <v>268</v>
       </c>
       <c r="I93" s="33"/>
     </row>
@@ -3896,14 +3884,14 @@
       <c r="C94" s="32"/>
       <c r="D94" s="32"/>
       <c r="E94" s="45" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F94" s="32"/>
       <c r="G94" s="45" t="s">
+        <v>269</v>
+      </c>
+      <c r="H94" s="45" t="s">
         <v>270</v>
-      </c>
-      <c r="H94" s="45" t="s">
-        <v>271</v>
       </c>
       <c r="I94" s="33"/>
     </row>
@@ -3912,91 +3900,91 @@
       <c r="B95" s="31"/>
       <c r="C95" s="32"/>
       <c r="D95" s="32"/>
-      <c r="E95" s="45" t="s">
-        <v>277</v>
+      <c r="E95" s="53" t="s">
+        <v>274</v>
       </c>
       <c r="F95" s="32"/>
       <c r="G95" s="45" t="s">
+        <v>269</v>
+      </c>
+      <c r="H95" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="H95" s="45" t="s">
-        <v>271</v>
-      </c>
       <c r="I95" s="33"/>
     </row>
-    <row r="96" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="30"/>
-      <c r="B96" s="31"/>
+    <row r="96" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="B96" s="51" t="s">
+        <v>275</v>
+      </c>
       <c r="C96" s="32"/>
-      <c r="D96" s="32"/>
-      <c r="E96" s="45" t="s">
-        <v>272</v>
-      </c>
-      <c r="F96" s="32"/>
+      <c r="D96" s="45" t="s">
+        <v>276</v>
+      </c>
+      <c r="E96" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F96" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G96" s="45" t="s">
-        <v>273</v>
+        <v>64</v>
       </c>
       <c r="H96" s="45" t="s">
-        <v>274</v>
+        <v>74</v>
       </c>
       <c r="I96" s="33"/>
     </row>
-    <row r="97" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A97" s="30"/>
       <c r="B97" s="31"/>
       <c r="C97" s="32"/>
       <c r="D97" s="32"/>
-      <c r="E97" s="53" t="s">
-        <v>278</v>
+      <c r="E97" s="32" t="s">
+        <v>277</v>
       </c>
       <c r="F97" s="32"/>
       <c r="G97" s="45" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="H97" s="45" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="I97" s="33"/>
     </row>
-    <row r="98" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="B98" s="51" t="s">
-        <v>279</v>
-      </c>
+    <row r="98" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A98" s="30"/>
+      <c r="B98" s="31"/>
       <c r="C98" s="32"/>
-      <c r="D98" s="45" t="s">
+      <c r="D98" s="32"/>
+      <c r="E98" s="54" t="s">
         <v>280</v>
       </c>
-      <c r="E98" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="F98" s="47" t="s">
-        <v>63</v>
-      </c>
+      <c r="F98" s="32"/>
       <c r="G98" s="45" t="s">
-        <v>64</v>
+        <v>281</v>
       </c>
       <c r="H98" s="45" t="s">
-        <v>74</v>
+        <v>282</v>
       </c>
       <c r="I98" s="33"/>
     </row>
-    <row r="99" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A99" s="30"/>
       <c r="B99" s="31"/>
       <c r="C99" s="32"/>
       <c r="D99" s="32"/>
-      <c r="E99" s="32" t="s">
-        <v>281</v>
+      <c r="E99" s="45" t="s">
+        <v>283</v>
       </c>
       <c r="F99" s="32"/>
       <c r="G99" s="45" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="H99" s="45" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="I99" s="33"/>
     </row>
@@ -4006,107 +3994,115 @@
       <c r="C100" s="32"/>
       <c r="D100" s="32"/>
       <c r="E100" s="54" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F100" s="32"/>
       <c r="G100" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="H100" s="45" t="s">
         <v>285</v>
       </c>
-      <c r="H100" s="45" t="s">
-        <v>286</v>
-      </c>
       <c r="I100" s="33"/>
     </row>
-    <row r="101" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A101" s="30"/>
-      <c r="B101" s="31"/>
+    <row r="101" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="B101" s="51" t="s">
+        <v>287</v>
+      </c>
       <c r="C101" s="32"/>
-      <c r="D101" s="32"/>
+      <c r="D101" s="45" t="s">
+        <v>288</v>
+      </c>
       <c r="E101" s="45" t="s">
-        <v>287</v>
-      </c>
-      <c r="F101" s="32"/>
+        <v>62</v>
+      </c>
+      <c r="F101" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G101" s="45" t="s">
-        <v>288</v>
+        <v>64</v>
       </c>
       <c r="H101" s="45" t="s">
-        <v>289</v>
+        <v>74</v>
       </c>
       <c r="I101" s="33"/>
     </row>
-    <row r="102" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A102" s="30"/>
       <c r="B102" s="31"/>
       <c r="C102" s="32"/>
       <c r="D102" s="32"/>
-      <c r="E102" s="54" t="s">
-        <v>290</v>
+      <c r="E102" s="45" t="s">
+        <v>289</v>
       </c>
       <c r="F102" s="32"/>
       <c r="G102" s="45" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="H102" s="45" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="I102" s="33"/>
     </row>
-    <row r="103" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="B103" s="51" t="s">
-        <v>291</v>
-      </c>
+    <row r="103" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="A103" s="30"/>
+      <c r="B103" s="31"/>
       <c r="C103" s="32"/>
-      <c r="D103" s="45" t="s">
+      <c r="D103" s="32"/>
+      <c r="E103" s="45" t="s">
         <v>292</v>
       </c>
-      <c r="E103" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="F103" s="47" t="s">
-        <v>63</v>
-      </c>
+      <c r="F103" s="32"/>
       <c r="G103" s="45" t="s">
-        <v>64</v>
+        <v>293</v>
       </c>
       <c r="H103" s="45" t="s">
-        <v>74</v>
+        <v>294</v>
       </c>
       <c r="I103" s="33"/>
     </row>
-    <row r="104" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A104" s="30"/>
       <c r="B104" s="31"/>
       <c r="C104" s="32"/>
       <c r="D104" s="32"/>
-      <c r="E104" s="45" t="s">
-        <v>293</v>
+      <c r="E104" s="54" t="s">
+        <v>297</v>
       </c>
       <c r="F104" s="32"/>
       <c r="G104" s="45" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H104" s="45" t="s">
         <v>295</v>
       </c>
       <c r="I104" s="33"/>
     </row>
-    <row r="105" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="A105" s="30"/>
-      <c r="B105" s="31"/>
+    <row r="105" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="B105" s="51" t="s">
+        <v>298</v>
+      </c>
       <c r="C105" s="32"/>
-      <c r="D105" s="32"/>
+      <c r="D105" s="45" t="s">
+        <v>299</v>
+      </c>
       <c r="E105" s="45" t="s">
-        <v>296</v>
-      </c>
-      <c r="F105" s="32"/>
+        <v>62</v>
+      </c>
+      <c r="F105" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G105" s="45" t="s">
-        <v>297</v>
+        <v>64</v>
       </c>
       <c r="H105" s="45" t="s">
-        <v>298</v>
+        <v>74</v>
       </c>
       <c r="I105" s="33"/>
     </row>
@@ -4115,133 +4111,125 @@
       <c r="B106" s="31"/>
       <c r="C106" s="32"/>
       <c r="D106" s="32"/>
-      <c r="E106" s="54" t="s">
-        <v>301</v>
+      <c r="E106" s="45" t="s">
+        <v>300</v>
       </c>
       <c r="F106" s="32"/>
       <c r="G106" s="45" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H106" s="45" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="I106" s="33"/>
     </row>
-    <row r="107" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="B107" s="51" t="s">
-        <v>302</v>
-      </c>
+    <row r="107" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A107" s="30"/>
+      <c r="B107" s="31"/>
       <c r="C107" s="32"/>
-      <c r="D107" s="45" t="s">
-        <v>303</v>
-      </c>
-      <c r="E107" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="F107" s="47" t="s">
-        <v>63</v>
-      </c>
+      <c r="D107" s="32"/>
+      <c r="E107" s="60" t="s">
+        <v>304</v>
+      </c>
+      <c r="F107" s="32"/>
       <c r="G107" s="45" t="s">
-        <v>64</v>
+        <v>305</v>
       </c>
       <c r="H107" s="45" t="s">
-        <v>74</v>
+        <v>306</v>
       </c>
       <c r="I107" s="33"/>
     </row>
-    <row r="108" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A108" s="30"/>
       <c r="B108" s="31"/>
       <c r="C108" s="32"/>
       <c r="D108" s="32"/>
-      <c r="E108" s="45" t="s">
-        <v>304</v>
+      <c r="E108" s="59" t="s">
+        <v>303</v>
       </c>
       <c r="F108" s="32"/>
       <c r="G108" s="45" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="H108" s="45" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="I108" s="33"/>
     </row>
-    <row r="109" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="30"/>
-      <c r="B109" s="31"/>
+    <row r="109" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="B109" s="51" t="s">
+        <v>309</v>
+      </c>
       <c r="C109" s="32"/>
-      <c r="D109" s="32"/>
-      <c r="E109" s="65" t="s">
-        <v>308</v>
-      </c>
-      <c r="F109" s="32"/>
+      <c r="D109" s="45" t="s">
+        <v>310</v>
+      </c>
+      <c r="E109" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="F109" s="47" t="s">
+        <v>63</v>
+      </c>
       <c r="G109" s="45" t="s">
-        <v>309</v>
+        <v>64</v>
       </c>
       <c r="H109" s="45" t="s">
-        <v>310</v>
+        <v>74</v>
       </c>
       <c r="I109" s="33"/>
     </row>
-    <row r="110" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A110" s="30"/>
-      <c r="B110" s="31"/>
+    <row r="110" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="58"/>
+      <c r="B110" s="51"/>
       <c r="C110" s="32"/>
-      <c r="D110" s="32"/>
-      <c r="E110" s="64" t="s">
-        <v>307</v>
-      </c>
-      <c r="F110" s="32"/>
+      <c r="D110" s="45"/>
+      <c r="E110" s="45" t="s">
+        <v>311</v>
+      </c>
+      <c r="F110" s="47"/>
       <c r="G110" s="45" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H110" s="45" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="I110" s="33"/>
     </row>
-    <row r="111" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="B111" s="51" t="s">
-        <v>313</v>
-      </c>
+    <row r="111" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A111" s="58"/>
+      <c r="B111" s="51"/>
       <c r="C111" s="32"/>
-      <c r="D111" s="45" t="s">
-        <v>314</v>
-      </c>
-      <c r="E111" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="F111" s="47" t="s">
-        <v>63</v>
-      </c>
+      <c r="D111" s="45"/>
+      <c r="E111" s="54" t="s">
+        <v>315</v>
+      </c>
+      <c r="F111" s="47"/>
       <c r="G111" s="45" t="s">
-        <v>64</v>
+        <v>316</v>
       </c>
       <c r="H111" s="45" t="s">
-        <v>74</v>
+        <v>317</v>
       </c>
       <c r="I111" s="33"/>
     </row>
-    <row r="112" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A112" s="58"/>
       <c r="B112" s="51"/>
       <c r="C112" s="32"/>
       <c r="D112" s="45"/>
       <c r="E112" s="45" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="F112" s="47"/>
       <c r="G112" s="45" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H112" s="45" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="I112" s="33"/>
     </row>
@@ -4255,68 +4243,34 @@
       </c>
       <c r="F113" s="47"/>
       <c r="G113" s="45" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="H113" s="45" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="I113" s="33"/>
     </row>
-    <row r="114" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="A114" s="58"/>
-      <c r="B114" s="51"/>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="30"/>
+      <c r="B114" s="31"/>
       <c r="C114" s="32"/>
-      <c r="D114" s="45"/>
-      <c r="E114" s="45" t="s">
-        <v>324</v>
-      </c>
-      <c r="F114" s="47"/>
-      <c r="G114" s="45" t="s">
-        <v>318</v>
-      </c>
-      <c r="H114" s="45" t="s">
-        <v>322</v>
-      </c>
+      <c r="D114" s="32"/>
+      <c r="E114" s="32"/>
+      <c r="F114" s="32"/>
+      <c r="G114" s="32"/>
+      <c r="H114" s="32"/>
       <c r="I114" s="33"/>
     </row>
-    <row r="115" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A115" s="58"/>
-      <c r="B115" s="51"/>
-      <c r="C115" s="32"/>
-      <c r="D115" s="45"/>
-      <c r="E115" s="54" t="s">
-        <v>323</v>
-      </c>
-      <c r="F115" s="47"/>
-      <c r="G115" s="45" t="s">
-        <v>318</v>
-      </c>
-      <c r="H115" s="45" t="s">
-        <v>322</v>
-      </c>
-      <c r="I115" s="33"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="30"/>
-      <c r="B116" s="31"/>
-      <c r="C116" s="32"/>
-      <c r="D116" s="32"/>
-      <c r="E116" s="32"/>
-      <c r="F116" s="32"/>
-      <c r="G116" s="32"/>
-      <c r="H116" s="32"/>
-      <c r="I116" s="33"/>
-    </row>
-    <row r="117" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="34"/>
-      <c r="B117" s="35"/>
-      <c r="C117" s="36"/>
-      <c r="D117" s="36"/>
-      <c r="E117" s="36"/>
-      <c r="F117" s="36"/>
-      <c r="G117" s="36"/>
-      <c r="H117" s="36"/>
-      <c r="I117" s="37"/>
+    <row r="115" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="34"/>
+      <c r="B115" s="35"/>
+      <c r="C115" s="36"/>
+      <c r="D115" s="36"/>
+      <c r="E115" s="36"/>
+      <c r="F115" s="36"/>
+      <c r="G115" s="36"/>
+      <c r="H115" s="36"/>
+      <c r="I115" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4329,20 +4283,20 @@
     <hyperlink ref="F16" r:id="rId2" xr:uid="{E4466D79-2CE6-4A09-9629-10C6FB0938C5}"/>
     <hyperlink ref="F21" r:id="rId3" xr:uid="{5E7C1B99-3701-4972-9537-AE0A96C8E1B9}"/>
     <hyperlink ref="F27" r:id="rId4" xr:uid="{42A4B507-5FFD-4AFD-BD89-FFF0CEB1EBCA}"/>
-    <hyperlink ref="F35" r:id="rId5" xr:uid="{99513BB9-1EF9-4351-B914-46372C3CDBF5}"/>
-    <hyperlink ref="F40" r:id="rId6" xr:uid="{0A2DC24E-A9AB-434E-A812-CFD454AFD884}"/>
-    <hyperlink ref="F46" r:id="rId7" xr:uid="{D75FD608-4DB9-465F-8C2F-F6010FA95860}"/>
-    <hyperlink ref="F51" r:id="rId8" xr:uid="{F18D8A63-6F97-49C5-9C3F-1A5CA3B7905E}"/>
-    <hyperlink ref="F58" r:id="rId9" xr:uid="{B93C7181-8F67-4156-9737-1E62E8E118DA}"/>
-    <hyperlink ref="F65" r:id="rId10" xr:uid="{38C773A1-3BC7-4C3B-86E6-BF32F3AD4C6E}"/>
-    <hyperlink ref="F70" r:id="rId11" xr:uid="{7F4F6A8C-AA17-4340-A40E-12303FEF29BC}"/>
-    <hyperlink ref="F77" r:id="rId12" xr:uid="{628B29C5-A280-4C65-B16F-9229BD446432}"/>
-    <hyperlink ref="F82" r:id="rId13" xr:uid="{0F214E2E-2D9B-48C2-AA50-AA0E7B1CD847}"/>
-    <hyperlink ref="F87" r:id="rId14" xr:uid="{018D8B70-E240-478A-877C-1B64E2B66707}"/>
-    <hyperlink ref="F98" r:id="rId15" xr:uid="{33E612D4-2082-4338-AAF2-0EE5AFFF32D1}"/>
-    <hyperlink ref="F103" r:id="rId16" xr:uid="{B72CDD78-A935-497F-9CB9-CA194A8DA39D}"/>
-    <hyperlink ref="F107" r:id="rId17" xr:uid="{757F55F1-53F2-4ABC-9889-CDDE44904BFB}"/>
-    <hyperlink ref="F111" r:id="rId18" xr:uid="{1033D818-4443-48C9-B429-21937673AF2E}"/>
+    <hyperlink ref="F33" r:id="rId5" xr:uid="{99513BB9-1EF9-4351-B914-46372C3CDBF5}"/>
+    <hyperlink ref="F38" r:id="rId6" xr:uid="{0A2DC24E-A9AB-434E-A812-CFD454AFD884}"/>
+    <hyperlink ref="F44" r:id="rId7" xr:uid="{D75FD608-4DB9-465F-8C2F-F6010FA95860}"/>
+    <hyperlink ref="F49" r:id="rId8" xr:uid="{F18D8A63-6F97-49C5-9C3F-1A5CA3B7905E}"/>
+    <hyperlink ref="F56" r:id="rId9" xr:uid="{B93C7181-8F67-4156-9737-1E62E8E118DA}"/>
+    <hyperlink ref="F63" r:id="rId10" xr:uid="{38C773A1-3BC7-4C3B-86E6-BF32F3AD4C6E}"/>
+    <hyperlink ref="F68" r:id="rId11" xr:uid="{7F4F6A8C-AA17-4340-A40E-12303FEF29BC}"/>
+    <hyperlink ref="F75" r:id="rId12" xr:uid="{628B29C5-A280-4C65-B16F-9229BD446432}"/>
+    <hyperlink ref="F80" r:id="rId13" xr:uid="{0F214E2E-2D9B-48C2-AA50-AA0E7B1CD847}"/>
+    <hyperlink ref="F85" r:id="rId14" xr:uid="{018D8B70-E240-478A-877C-1B64E2B66707}"/>
+    <hyperlink ref="F96" r:id="rId15" xr:uid="{33E612D4-2082-4338-AAF2-0EE5AFFF32D1}"/>
+    <hyperlink ref="F101" r:id="rId16" xr:uid="{B72CDD78-A935-497F-9CB9-CA194A8DA39D}"/>
+    <hyperlink ref="F105" r:id="rId17" xr:uid="{757F55F1-53F2-4ABC-9889-CDDE44904BFB}"/>
+    <hyperlink ref="F109" r:id="rId18" xr:uid="{1033D818-4443-48C9-B429-21937673AF2E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>

</xml_diff>

<commit_message>
I changed source file and some code
</commit_message>
<xml_diff>
--- a/source_file/jquery_testscenario.xlsx
+++ b/source_file/jquery_testscenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gturd\IdeaProjects\FirstAssignment\source_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD56A360-00F1-4469-B3CC-B4CF482C4B25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0FE29F-D286-446E-8BF0-6072760D97A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{CE714CED-6ED2-47BF-9249-83F3ACACC2F2}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="333">
   <si>
     <t>Project Name:</t>
   </si>
@@ -232,21 +232,12 @@
     <t>Click on the Draggable link</t>
   </si>
   <si>
-    <t>The Drag me around tab should be draging around within that window or that frame</t>
-  </si>
-  <si>
     <t>Test Scenario/Description</t>
   </si>
   <si>
     <t>Test Case</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Draggable page</t>
-  </si>
-  <si>
-    <t>Click on the Drag me around tab and drag around within the window</t>
-  </si>
-  <si>
     <t>Draggable page should be displayed</t>
   </si>
   <si>
@@ -256,9 +247,6 @@
     <t>Draggable page is displayed</t>
   </si>
   <si>
-    <t>Drag me around tab is draged around within that window</t>
-  </si>
-  <si>
     <t>Verify Drag me around tab move to another location</t>
   </si>
   <si>
@@ -274,9 +262,6 @@
     <t>Droppable</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Droppable page</t>
-  </si>
-  <si>
     <t>Click on the Droppable link</t>
   </si>
   <si>
@@ -310,9 +295,6 @@
     <t>Resizable</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Resizable page</t>
-  </si>
-  <si>
     <t>Click on the Resizable link</t>
   </si>
   <si>
@@ -358,9 +340,6 @@
     <t>Selectable</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Selectable page</t>
-  </si>
-  <si>
     <t>Click on the Selectable link</t>
   </si>
   <si>
@@ -406,9 +385,6 @@
     <t>The links are clicked one by one</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Sortable page</t>
-  </si>
-  <si>
     <t>Click on the Sortable link</t>
   </si>
   <si>
@@ -442,9 +418,6 @@
     <t>Check the Accordion Functionality</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Accordion page</t>
-  </si>
-  <si>
     <t>Click on the Accordion link</t>
   </si>
   <si>
@@ -484,9 +457,6 @@
     <t>Autocomplete</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Autocomplete page</t>
-  </si>
-  <si>
     <t>Click on the Autocomplete link</t>
   </si>
   <si>
@@ -517,9 +487,6 @@
     <t>Verify the value is displayed</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Button page</t>
-  </si>
-  <si>
     <t>Click on the Button link</t>
   </si>
   <si>
@@ -649,9 +616,6 @@
     <t>TC-011</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Controlgroup page</t>
-  </si>
-  <si>
     <t>Click on the Datepicker link</t>
   </si>
   <si>
@@ -703,12 +667,6 @@
     <t>TC-012</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Datepicker page</t>
-  </si>
-  <si>
-    <t>The user should be able to open the browser and do some actions on the Dialog page</t>
-  </si>
-  <si>
     <t>Click on the Dialog link</t>
   </si>
   <si>
@@ -748,9 +706,6 @@
     <t>TC-013</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Menu page</t>
-  </si>
-  <si>
     <t>Click on the Menu link</t>
   </si>
   <si>
@@ -784,9 +739,6 @@
     <t>TC-014</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Selectmenu page</t>
-  </si>
-  <si>
     <t>Click on the Selectmenu link</t>
   </si>
   <si>
@@ -856,9 +808,6 @@
     <t>TC-015</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Slider page</t>
-  </si>
-  <si>
     <t>Click on the Slider link</t>
   </si>
   <si>
@@ -892,9 +841,6 @@
     <t>TC-016</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Spinner page</t>
-  </si>
-  <si>
     <t>Click on the Spinner link</t>
   </si>
   <si>
@@ -925,9 +871,6 @@
     <t>TC-017</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Tabs page</t>
-  </si>
-  <si>
     <t>Click on the Tabs link</t>
   </si>
   <si>
@@ -958,9 +901,6 @@
     <t>TC-018</t>
   </si>
   <si>
-    <t>The user should be able to open the browser and do some actions on the Tooltip page</t>
-  </si>
-  <si>
     <t>Click on the Tooltip link</t>
   </si>
   <si>
@@ -1022,6 +962,69 @@
   </si>
   <si>
     <t>The Autocomplete link shoul be clicked and Autocomplete page should be displayed</t>
+  </si>
+  <si>
+    <t>Click on the Drag me around tab and drag the square move to another location then dropped within the window</t>
+  </si>
+  <si>
+    <t>The Drag me around tab should be draging the another location then dropped within that window or that frame</t>
+  </si>
+  <si>
+    <t>Drag me around tab is dropped to another location within that window</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and user should be able to change size of the object on the Resizable page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and user should be able to drag the object drop to given location on the Droppable page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to move, resize and close the dialog window on the Dialog page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to select items on the Selectable page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to  drag the square move to another location on the Draggable page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to drag an item to reorder the location on the Sortable page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to displays collapsible content panels on the Accordion page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to automatically provides suggestions while you type into the field on the Autocomplete page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to click the widget buttons or CSS buttons on the Button page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to check the Radio button and Checkbox button on the Button page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to control the various toolbar on the Controlgroup page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to select date from a popup or inline calendar on the Datepicker page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to navigate to an item for configuration, disabled  and nested on the Menu page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to replace select element on the Selectmenu page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to drag a handle to select a numeric value on the Slider page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to input numeric value text field on the Spinner page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to click tabs to swap between content on the Tabs page</t>
+  </si>
+  <si>
+    <t>The user should be able to open the browser and should be able to show additional information on context field on the Tooltip page</t>
   </si>
 </sst>
 </file>
@@ -2168,7 +2171,7 @@
   <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,7 +2317,7 @@
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" s="24" t="s">
         <v>10</v>
@@ -2323,7 +2326,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" s="24" t="s">
         <v>12</v>
@@ -2341,7 +2344,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
         <v>22</v>
       </c>
@@ -2352,7 +2355,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>71</v>
+        <v>319</v>
       </c>
       <c r="E11" s="28" t="s">
         <v>62</v>
@@ -2364,7 +2367,7 @@
         <v>64</v>
       </c>
       <c r="H11" s="46" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I11" s="29"/>
     </row>
@@ -2378,10 +2381,10 @@
       </c>
       <c r="F12" s="32"/>
       <c r="G12" s="45" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="H12" s="45" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="I12" s="33"/>
     </row>
@@ -2391,31 +2394,31 @@
       <c r="C13" s="32"/>
       <c r="D13" s="45"/>
       <c r="E13" s="54" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="45" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H13" s="45" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I13" s="33"/>
     </row>
-    <row r="14" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
       <c r="B14" s="31"/>
       <c r="C14" s="32"/>
       <c r="D14" s="32"/>
       <c r="E14" s="45" t="s">
-        <v>72</v>
+        <v>312</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="45" t="s">
-        <v>68</v>
+        <v>313</v>
       </c>
       <c r="H14" s="45" t="s">
-        <v>76</v>
+        <v>314</v>
       </c>
       <c r="I14" s="33"/>
     </row>
@@ -2425,29 +2428,29 @@
       <c r="C15" s="32"/>
       <c r="D15" s="32"/>
       <c r="E15" s="54" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="45" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H15" s="45" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I15" s="33"/>
     </row>
-    <row r="16" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A16" s="49" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D16" s="45" t="s">
-        <v>82</v>
+        <v>316</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>62</v>
@@ -2459,7 +2462,7 @@
         <v>64</v>
       </c>
       <c r="H16" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I16" s="33"/>
     </row>
@@ -2469,14 +2472,14 @@
       <c r="C17" s="32"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="45" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="H17" s="45" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="I17" s="33"/>
     </row>
@@ -2486,14 +2489,14 @@
       <c r="C18" s="32"/>
       <c r="D18" s="32"/>
       <c r="E18" s="54" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="45" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H18" s="45" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I18" s="33"/>
     </row>
@@ -2503,14 +2506,14 @@
       <c r="C19" s="32"/>
       <c r="D19" s="32"/>
       <c r="E19" s="45" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="45" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H19" s="45" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I19" s="33"/>
     </row>
@@ -2520,29 +2523,29 @@
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
       <c r="E20" s="54" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="45" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H20" s="45" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I20" s="33"/>
     </row>
-    <row r="21" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A21" s="49" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C21" s="53" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D21" s="45" t="s">
-        <v>94</v>
+        <v>315</v>
       </c>
       <c r="E21" s="32" t="s">
         <v>62</v>
@@ -2554,7 +2557,7 @@
         <v>64</v>
       </c>
       <c r="H21" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I21" s="33"/>
     </row>
@@ -2564,14 +2567,14 @@
       <c r="C22" s="32"/>
       <c r="D22" s="32"/>
       <c r="E22" s="32" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="45" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H22" s="45" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I22" s="33"/>
     </row>
@@ -2581,14 +2584,14 @@
       <c r="C23" s="32"/>
       <c r="D23" s="32"/>
       <c r="E23" s="54" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="45" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="H23" s="45" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I23" s="33"/>
     </row>
@@ -2598,14 +2601,14 @@
       <c r="C24" s="32"/>
       <c r="D24" s="32"/>
       <c r="E24" s="45" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="45" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="H24" s="45" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I24" s="33"/>
     </row>
@@ -2615,14 +2618,14 @@
       <c r="C25" s="32"/>
       <c r="D25" s="32"/>
       <c r="E25" s="54" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="45" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="H25" s="45" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I25" s="33"/>
     </row>
@@ -2632,29 +2635,29 @@
       <c r="C26" s="32"/>
       <c r="D26" s="32"/>
       <c r="E26" s="32" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="45" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="H26" s="45" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="I26" s="33"/>
     </row>
-    <row r="27" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A27" s="49" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C27" s="53" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D27" s="45" t="s">
-        <v>110</v>
+        <v>318</v>
       </c>
       <c r="E27" s="32" t="s">
         <v>62</v>
@@ -2666,7 +2669,7 @@
         <v>64</v>
       </c>
       <c r="H27" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I27" s="33"/>
     </row>
@@ -2676,14 +2679,14 @@
       <c r="C28" s="32"/>
       <c r="D28" s="32"/>
       <c r="E28" s="32" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="F28" s="32"/>
       <c r="G28" s="45" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="H28" s="45" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="I28" s="33"/>
     </row>
@@ -2693,14 +2696,14 @@
       <c r="C29" s="32"/>
       <c r="D29" s="32"/>
       <c r="E29" s="54" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F29" s="32"/>
       <c r="G29" s="45" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="H29" s="45" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="I29" s="33"/>
     </row>
@@ -2710,14 +2713,14 @@
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
       <c r="E30" s="45" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F30" s="32"/>
       <c r="G30" s="45" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H30" s="45" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="I30" s="33"/>
     </row>
@@ -2727,14 +2730,14 @@
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
       <c r="E31" s="53" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F31" s="32"/>
       <c r="G31" s="45" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="H31" s="45" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="I31" s="33"/>
     </row>
@@ -2744,29 +2747,29 @@
       <c r="C32" s="32"/>
       <c r="D32" s="32"/>
       <c r="E32" s="45" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F32" s="32"/>
       <c r="G32" s="45" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="H32" s="45" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="I32" s="33"/>
     </row>
-    <row r="33" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A33" s="49" t="s">
         <v>26</v>
       </c>
       <c r="B33" s="51" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C33" s="53" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D33" s="45" t="s">
-        <v>126</v>
+        <v>320</v>
       </c>
       <c r="E33" s="32" t="s">
         <v>62</v>
@@ -2778,7 +2781,7 @@
         <v>64</v>
       </c>
       <c r="H33" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I33" s="33"/>
     </row>
@@ -2788,14 +2791,14 @@
       <c r="C34" s="32"/>
       <c r="D34" s="32"/>
       <c r="E34" s="32" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F34" s="32"/>
       <c r="G34" s="45" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="H34" s="45" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="I34" s="33"/>
     </row>
@@ -2805,14 +2808,14 @@
       <c r="C35" s="32"/>
       <c r="D35" s="32"/>
       <c r="E35" s="54" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F35" s="32"/>
       <c r="G35" s="45" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="H35" s="45" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="I35" s="33"/>
     </row>
@@ -2822,14 +2825,14 @@
       <c r="C36" s="32"/>
       <c r="D36" s="32"/>
       <c r="E36" s="45" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F36" s="32"/>
       <c r="G36" s="45" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="H36" s="45" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="I36" s="33"/>
     </row>
@@ -2839,29 +2842,29 @@
       <c r="C37" s="32"/>
       <c r="D37" s="32"/>
       <c r="E37" s="54" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F37" s="32"/>
       <c r="G37" s="45" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="H37" s="45" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="I37" s="33"/>
     </row>
-    <row r="38" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A38" s="49" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B38" s="51" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C38" s="53" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D38" s="45" t="s">
-        <v>138</v>
+        <v>321</v>
       </c>
       <c r="E38" s="32" t="s">
         <v>62</v>
@@ -2873,7 +2876,7 @@
         <v>64</v>
       </c>
       <c r="H38" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I38" s="33"/>
     </row>
@@ -2883,14 +2886,14 @@
       <c r="C39" s="32"/>
       <c r="D39" s="32"/>
       <c r="E39" s="32" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F39" s="32"/>
       <c r="G39" s="45" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="H39" s="45" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="I39" s="33"/>
     </row>
@@ -2900,14 +2903,14 @@
       <c r="C40" s="32"/>
       <c r="D40" s="32"/>
       <c r="E40" s="54" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F40" s="32"/>
       <c r="G40" s="45" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="H40" s="45" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="I40" s="33"/>
     </row>
@@ -2917,14 +2920,14 @@
       <c r="C41" s="32"/>
       <c r="D41" s="32"/>
       <c r="E41" s="45" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F41" s="32"/>
       <c r="G41" s="55" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="H41" s="45" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="I41" s="33"/>
     </row>
@@ -2934,14 +2937,14 @@
       <c r="C42" s="32"/>
       <c r="D42" s="32"/>
       <c r="E42" s="54" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F42" s="32"/>
       <c r="G42" s="45" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="H42" s="45" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="I42" s="33"/>
     </row>
@@ -2951,29 +2954,29 @@
       <c r="C43" s="32"/>
       <c r="D43" s="32"/>
       <c r="E43" s="32" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F43" s="32"/>
       <c r="G43" s="45" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="H43" s="45" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="I43" s="33"/>
     </row>
-    <row r="44" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="102" x14ac:dyDescent="0.25">
       <c r="A44" s="49" t="s">
         <v>28</v>
       </c>
       <c r="B44" s="51" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C44" s="53" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D44" s="45" t="s">
-        <v>152</v>
+        <v>322</v>
       </c>
       <c r="E44" s="32" t="s">
         <v>62</v>
@@ -2985,7 +2988,7 @@
         <v>64</v>
       </c>
       <c r="H44" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I44" s="33"/>
     </row>
@@ -2995,14 +2998,14 @@
       <c r="C45" s="32"/>
       <c r="D45" s="32"/>
       <c r="E45" s="45" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="F45" s="32"/>
       <c r="G45" s="45" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="H45" s="45" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="I45" s="33"/>
     </row>
@@ -3012,14 +3015,14 @@
       <c r="C46" s="32"/>
       <c r="D46" s="32"/>
       <c r="E46" s="54" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F46" s="32"/>
       <c r="G46" s="45" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="H46" s="45" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="I46" s="33"/>
     </row>
@@ -3029,14 +3032,14 @@
       <c r="C47" s="32"/>
       <c r="D47" s="32"/>
       <c r="E47" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="F47" s="32"/>
       <c r="G47" s="45" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H47" s="45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="I47" s="33"/>
     </row>
@@ -3046,27 +3049,27 @@
       <c r="C48" s="32"/>
       <c r="D48" s="32"/>
       <c r="E48" s="54" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="F48" s="32"/>
       <c r="G48" s="45" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="H48" s="45" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="I48" s="33"/>
     </row>
-    <row r="49" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A49" s="49" t="s">
         <v>29</v>
       </c>
       <c r="B49" s="51" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C49" s="32"/>
       <c r="D49" s="45" t="s">
-        <v>163</v>
+        <v>323</v>
       </c>
       <c r="E49" s="32" t="s">
         <v>62</v>
@@ -3078,7 +3081,7 @@
         <v>64</v>
       </c>
       <c r="H49" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I49" s="33"/>
     </row>
@@ -3088,14 +3091,14 @@
       <c r="C50" s="32"/>
       <c r="D50" s="32"/>
       <c r="E50" s="32" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="F50" s="32"/>
       <c r="G50" s="45" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="H50" s="45" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="I50" s="33"/>
     </row>
@@ -3105,14 +3108,14 @@
       <c r="C51" s="32"/>
       <c r="D51" s="32"/>
       <c r="E51" s="54" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F51" s="32"/>
       <c r="G51" s="45" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="H51" s="45" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="I51" s="33"/>
     </row>
@@ -3122,14 +3125,14 @@
       <c r="C52" s="32"/>
       <c r="D52" s="32"/>
       <c r="E52" s="45" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="F52" s="32"/>
       <c r="G52" s="45" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="H52" s="45" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="I52" s="33"/>
     </row>
@@ -3139,14 +3142,14 @@
       <c r="C53" s="32"/>
       <c r="D53" s="32"/>
       <c r="E53" s="54" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="F53" s="32"/>
       <c r="G53" s="45" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="H53" s="45" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="I53" s="33"/>
     </row>
@@ -3156,14 +3159,14 @@
       <c r="C54" s="32"/>
       <c r="D54" s="32"/>
       <c r="E54" s="45" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="F54" s="32"/>
       <c r="G54" s="45" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="H54" s="45" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="I54" s="33"/>
     </row>
@@ -3173,27 +3176,27 @@
       <c r="C55" s="32"/>
       <c r="D55" s="32"/>
       <c r="E55" s="54" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F55" s="32"/>
       <c r="G55" s="45" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="H55" s="45" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="I55" s="33"/>
     </row>
-    <row r="56" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A56" s="49" t="s">
         <v>30</v>
       </c>
       <c r="B56" s="51" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C56" s="32"/>
       <c r="D56" s="45" t="s">
-        <v>163</v>
+        <v>324</v>
       </c>
       <c r="E56" s="32" t="s">
         <v>62</v>
@@ -3205,7 +3208,7 @@
         <v>64</v>
       </c>
       <c r="H56" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I56" s="33"/>
     </row>
@@ -3215,14 +3218,14 @@
       <c r="C57" s="32"/>
       <c r="D57" s="32"/>
       <c r="E57" s="45" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="F57" s="32"/>
       <c r="G57" s="45" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="H57" s="45" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="I57" s="33"/>
     </row>
@@ -3232,14 +3235,14 @@
       <c r="C58" s="32"/>
       <c r="D58" s="32"/>
       <c r="E58" s="54" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F58" s="32"/>
       <c r="G58" s="45" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H58" s="45" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="I58" s="33"/>
     </row>
@@ -3249,14 +3252,14 @@
       <c r="C59" s="32"/>
       <c r="D59" s="32"/>
       <c r="E59" s="45" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="F59" s="32"/>
       <c r="G59" s="56" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="H59" s="45" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="I59" s="33"/>
     </row>
@@ -3266,14 +3269,14 @@
       <c r="C60" s="32"/>
       <c r="D60" s="32"/>
       <c r="E60" s="54" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="F60" s="32"/>
       <c r="G60" s="45" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="H60" s="45" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="I60" s="33"/>
     </row>
@@ -3283,14 +3286,14 @@
       <c r="C61" s="32"/>
       <c r="D61" s="32"/>
       <c r="E61" s="45" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="F61" s="32"/>
       <c r="G61" s="45" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="H61" s="45" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="I61" s="33"/>
     </row>
@@ -3300,27 +3303,27 @@
       <c r="C62" s="32"/>
       <c r="D62" s="32"/>
       <c r="E62" s="53" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="F62" s="32"/>
       <c r="G62" s="45" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="H62" s="45" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="I62" s="33"/>
     </row>
-    <row r="63" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A63" s="49" t="s">
         <v>31</v>
       </c>
       <c r="B63" s="57" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C63" s="32"/>
       <c r="D63" s="45" t="s">
-        <v>207</v>
+        <v>325</v>
       </c>
       <c r="E63" s="32" t="s">
         <v>62</v>
@@ -3332,7 +3335,7 @@
         <v>64</v>
       </c>
       <c r="H63" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I63" s="33"/>
     </row>
@@ -3342,14 +3345,14 @@
       <c r="C64" s="32"/>
       <c r="D64" s="32"/>
       <c r="E64" s="45" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="F64" s="32"/>
       <c r="G64" s="45" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="H64" s="45" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="I64" s="33"/>
     </row>
@@ -3359,14 +3362,14 @@
       <c r="C65" s="32"/>
       <c r="D65" s="32"/>
       <c r="E65" s="54" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="F65" s="32"/>
       <c r="G65" s="45" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="H65" s="45" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="I65" s="33"/>
     </row>
@@ -3376,14 +3379,14 @@
       <c r="C66" s="32"/>
       <c r="D66" s="32"/>
       <c r="E66" s="45" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="F66" s="32"/>
       <c r="G66" s="45" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="H66" s="45" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="I66" s="33"/>
     </row>
@@ -3393,27 +3396,27 @@
       <c r="C67" s="32"/>
       <c r="D67" s="32"/>
       <c r="E67" s="54" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="F67" s="32"/>
       <c r="G67" s="45" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="H67" s="45" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="I67" s="33"/>
     </row>
-    <row r="68" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A68" s="58" t="s">
         <v>32</v>
       </c>
       <c r="B68" s="51" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C68" s="32"/>
       <c r="D68" s="45" t="s">
-        <v>225</v>
+        <v>326</v>
       </c>
       <c r="E68" s="32" t="s">
         <v>62</v>
@@ -3425,7 +3428,7 @@
         <v>64</v>
       </c>
       <c r="H68" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I68" s="33"/>
     </row>
@@ -3435,14 +3438,14 @@
       <c r="C69" s="32"/>
       <c r="D69" s="32"/>
       <c r="E69" s="32" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="F69" s="32"/>
       <c r="G69" s="45" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="H69" s="45" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="I69" s="33"/>
     </row>
@@ -3452,14 +3455,14 @@
       <c r="C70" s="32"/>
       <c r="D70" s="32"/>
       <c r="E70" s="54" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="F70" s="32"/>
       <c r="G70" s="45" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="H70" s="45" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="I70" s="33"/>
     </row>
@@ -3469,14 +3472,14 @@
       <c r="C71" s="32"/>
       <c r="D71" s="32"/>
       <c r="E71" s="45" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="F71" s="32"/>
       <c r="G71" s="45" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="H71" s="45" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="I71" s="33"/>
     </row>
@@ -3486,14 +3489,14 @@
       <c r="C72" s="32"/>
       <c r="D72" s="32"/>
       <c r="E72" s="45" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="F72" s="32"/>
       <c r="G72" s="45" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="H72" s="45" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="I72" s="33"/>
     </row>
@@ -3503,14 +3506,14 @@
       <c r="C73" s="32"/>
       <c r="D73" s="32"/>
       <c r="E73" s="45" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="F73" s="32"/>
       <c r="G73" s="45" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="H73" s="45" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I73" s="33"/>
     </row>
@@ -3520,27 +3523,27 @@
       <c r="C74" s="32"/>
       <c r="D74" s="32"/>
       <c r="E74" s="54" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="F74" s="32"/>
       <c r="G74" s="45" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="H74" s="45" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I74" s="33"/>
     </row>
-    <row r="75" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A75" s="58" t="s">
         <v>33</v>
       </c>
       <c r="B75" s="51" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="C75" s="32"/>
       <c r="D75" s="45" t="s">
-        <v>226</v>
+        <v>317</v>
       </c>
       <c r="E75" s="45" t="s">
         <v>62</v>
@@ -3552,7 +3555,7 @@
         <v>64</v>
       </c>
       <c r="H75" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I75" s="33"/>
     </row>
@@ -3562,14 +3565,14 @@
       <c r="C76" s="32"/>
       <c r="D76" s="32"/>
       <c r="E76" s="45" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="F76" s="32"/>
       <c r="G76" s="45" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="H76" s="45" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="I76" s="33"/>
     </row>
@@ -3579,14 +3582,14 @@
       <c r="C77" s="32"/>
       <c r="D77" s="32"/>
       <c r="E77" s="54" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="F77" s="32"/>
       <c r="G77" s="45" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="H77" s="45" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="I77" s="33"/>
     </row>
@@ -3596,14 +3599,14 @@
       <c r="C78" s="32"/>
       <c r="D78" s="32"/>
       <c r="E78" s="45" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="F78" s="32"/>
       <c r="G78" s="45" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="H78" s="45" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="I78" s="33"/>
     </row>
@@ -3613,27 +3616,27 @@
       <c r="C79" s="32"/>
       <c r="D79" s="32"/>
       <c r="E79" s="45" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="F79" s="32"/>
       <c r="G79" s="45" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="H79" s="45" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="I79" s="33"/>
     </row>
-    <row r="80" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A80" s="58" t="s">
         <v>34</v>
       </c>
       <c r="B80" s="51" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="C80" s="32"/>
       <c r="D80" s="45" t="s">
-        <v>240</v>
+        <v>327</v>
       </c>
       <c r="E80" s="45" t="s">
         <v>62</v>
@@ -3645,7 +3648,7 @@
         <v>64</v>
       </c>
       <c r="H80" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I80" s="33"/>
     </row>
@@ -3655,14 +3658,14 @@
       <c r="C81" s="32"/>
       <c r="D81" s="32"/>
       <c r="E81" s="45" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="F81" s="32"/>
       <c r="G81" s="45" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="H81" s="45" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="I81" s="33"/>
     </row>
@@ -3672,14 +3675,14 @@
       <c r="C82" s="32"/>
       <c r="D82" s="32"/>
       <c r="E82" s="54" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="F82" s="32"/>
       <c r="G82" s="45" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="H82" s="45" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="I82" s="33"/>
     </row>
@@ -3689,14 +3692,14 @@
       <c r="C83" s="32"/>
       <c r="D83" s="32"/>
       <c r="E83" s="45" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="F83" s="32"/>
       <c r="G83" s="45" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="H83" s="45" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="I83" s="33"/>
     </row>
@@ -3706,27 +3709,27 @@
       <c r="C84" s="32"/>
       <c r="D84" s="32"/>
       <c r="E84" s="54" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="F84" s="32"/>
       <c r="G84" s="45" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="H84" s="45" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="I84" s="33"/>
     </row>
-    <row r="85" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A85" s="58" t="s">
         <v>36</v>
       </c>
       <c r="B85" s="51" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C85" s="32"/>
       <c r="D85" s="45" t="s">
-        <v>252</v>
+        <v>328</v>
       </c>
       <c r="E85" s="32" t="s">
         <v>62</v>
@@ -3738,7 +3741,7 @@
         <v>64</v>
       </c>
       <c r="H85" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I85" s="33"/>
     </row>
@@ -3748,14 +3751,14 @@
       <c r="C86" s="32"/>
       <c r="D86" s="32"/>
       <c r="E86" s="32" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="F86" s="32"/>
       <c r="G86" s="45" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="H86" s="45" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="I86" s="33"/>
     </row>
@@ -3765,14 +3768,14 @@
       <c r="C87" s="32"/>
       <c r="D87" s="32"/>
       <c r="E87" s="54" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="F87" s="32"/>
       <c r="G87" s="45" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="H87" s="45" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="I87" s="33"/>
     </row>
@@ -3782,14 +3785,14 @@
       <c r="C88" s="32"/>
       <c r="D88" s="32"/>
       <c r="E88" s="45" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="F88" s="32"/>
       <c r="G88" s="45" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="H88" s="45" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="I88" s="33"/>
     </row>
@@ -3799,14 +3802,14 @@
       <c r="C89" s="32"/>
       <c r="D89" s="32"/>
       <c r="E89" s="45" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="F89" s="32"/>
       <c r="G89" s="45" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="H89" s="45" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="I89" s="33"/>
     </row>
@@ -3816,14 +3819,14 @@
       <c r="C90" s="32"/>
       <c r="D90" s="32"/>
       <c r="E90" s="45" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="F90" s="32"/>
       <c r="G90" s="45" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="H90" s="45" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="I90" s="33"/>
     </row>
@@ -3833,14 +3836,14 @@
       <c r="C91" s="32"/>
       <c r="D91" s="32"/>
       <c r="E91" s="45" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="F91" s="32"/>
       <c r="G91" s="45" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="H91" s="45" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="I91" s="33"/>
     </row>
@@ -3850,14 +3853,14 @@
       <c r="C92" s="32"/>
       <c r="D92" s="32"/>
       <c r="E92" s="45" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="F92" s="32"/>
       <c r="G92" s="45" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="H92" s="45" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="I92" s="33"/>
     </row>
@@ -3867,14 +3870,14 @@
       <c r="C93" s="32"/>
       <c r="D93" s="32"/>
       <c r="E93" s="45" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="F93" s="32"/>
       <c r="G93" s="45" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="H93" s="45" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="I93" s="33"/>
     </row>
@@ -3884,14 +3887,14 @@
       <c r="C94" s="32"/>
       <c r="D94" s="32"/>
       <c r="E94" s="45" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="F94" s="32"/>
       <c r="G94" s="45" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="H94" s="45" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="I94" s="33"/>
     </row>
@@ -3901,27 +3904,27 @@
       <c r="C95" s="32"/>
       <c r="D95" s="32"/>
       <c r="E95" s="53" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="F95" s="32"/>
       <c r="G95" s="45" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="H95" s="45" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="I95" s="33"/>
     </row>
-    <row r="96" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A96" s="58" t="s">
         <v>37</v>
       </c>
       <c r="B96" s="51" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="C96" s="32"/>
       <c r="D96" s="45" t="s">
-        <v>276</v>
+        <v>329</v>
       </c>
       <c r="E96" s="32" t="s">
         <v>62</v>
@@ -3933,7 +3936,7 @@
         <v>64</v>
       </c>
       <c r="H96" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I96" s="33"/>
     </row>
@@ -3943,14 +3946,14 @@
       <c r="C97" s="32"/>
       <c r="D97" s="32"/>
       <c r="E97" s="32" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="F97" s="32"/>
       <c r="G97" s="45" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="H97" s="45" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="I97" s="33"/>
     </row>
@@ -3960,14 +3963,14 @@
       <c r="C98" s="32"/>
       <c r="D98" s="32"/>
       <c r="E98" s="54" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="F98" s="32"/>
       <c r="G98" s="45" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="H98" s="45" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="I98" s="33"/>
     </row>
@@ -3977,14 +3980,14 @@
       <c r="C99" s="32"/>
       <c r="D99" s="32"/>
       <c r="E99" s="45" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F99" s="32"/>
       <c r="G99" s="45" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="H99" s="45" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="I99" s="33"/>
     </row>
@@ -3994,27 +3997,27 @@
       <c r="C100" s="32"/>
       <c r="D100" s="32"/>
       <c r="E100" s="54" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="F100" s="32"/>
       <c r="G100" s="45" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="H100" s="45" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="I100" s="33"/>
     </row>
-    <row r="101" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A101" s="58" t="s">
         <v>38</v>
       </c>
       <c r="B101" s="51" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="C101" s="32"/>
       <c r="D101" s="45" t="s">
-        <v>288</v>
+        <v>330</v>
       </c>
       <c r="E101" s="45" t="s">
         <v>62</v>
@@ -4026,7 +4029,7 @@
         <v>64</v>
       </c>
       <c r="H101" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I101" s="33"/>
     </row>
@@ -4036,14 +4039,14 @@
       <c r="C102" s="32"/>
       <c r="D102" s="32"/>
       <c r="E102" s="45" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="F102" s="32"/>
       <c r="G102" s="45" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="H102" s="45" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="I102" s="33"/>
     </row>
@@ -4053,14 +4056,14 @@
       <c r="C103" s="32"/>
       <c r="D103" s="32"/>
       <c r="E103" s="45" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="F103" s="32"/>
       <c r="G103" s="45" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="H103" s="45" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="I103" s="33"/>
     </row>
@@ -4070,27 +4073,27 @@
       <c r="C104" s="32"/>
       <c r="D104" s="32"/>
       <c r="E104" s="54" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="F104" s="32"/>
       <c r="G104" s="45" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="H104" s="45" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="I104" s="33"/>
     </row>
-    <row r="105" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A105" s="58" t="s">
         <v>39</v>
       </c>
       <c r="B105" s="51" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="C105" s="32"/>
       <c r="D105" s="45" t="s">
-        <v>299</v>
+        <v>331</v>
       </c>
       <c r="E105" s="45" t="s">
         <v>62</v>
@@ -4102,7 +4105,7 @@
         <v>64</v>
       </c>
       <c r="H105" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I105" s="33"/>
     </row>
@@ -4112,14 +4115,14 @@
       <c r="C106" s="32"/>
       <c r="D106" s="32"/>
       <c r="E106" s="45" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="F106" s="32"/>
       <c r="G106" s="45" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
       <c r="H106" s="45" t="s">
-        <v>302</v>
+        <v>283</v>
       </c>
       <c r="I106" s="33"/>
     </row>
@@ -4129,14 +4132,14 @@
       <c r="C107" s="32"/>
       <c r="D107" s="32"/>
       <c r="E107" s="60" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
       <c r="F107" s="32"/>
       <c r="G107" s="45" t="s">
-        <v>305</v>
+        <v>286</v>
       </c>
       <c r="H107" s="45" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="I107" s="33"/>
     </row>
@@ -4146,27 +4149,27 @@
       <c r="C108" s="32"/>
       <c r="D108" s="32"/>
       <c r="E108" s="59" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="F108" s="32"/>
       <c r="G108" s="45" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="H108" s="45" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
       <c r="I108" s="33"/>
     </row>
-    <row r="109" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A109" s="58" t="s">
         <v>40</v>
       </c>
       <c r="B109" s="51" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="C109" s="32"/>
       <c r="D109" s="45" t="s">
-        <v>310</v>
+        <v>332</v>
       </c>
       <c r="E109" s="45" t="s">
         <v>62</v>
@@ -4178,7 +4181,7 @@
         <v>64</v>
       </c>
       <c r="H109" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I109" s="33"/>
     </row>
@@ -4188,14 +4191,14 @@
       <c r="C110" s="32"/>
       <c r="D110" s="45"/>
       <c r="E110" s="45" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="F110" s="47"/>
       <c r="G110" s="45" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="H110" s="45" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="I110" s="33"/>
     </row>
@@ -4205,14 +4208,14 @@
       <c r="C111" s="32"/>
       <c r="D111" s="45"/>
       <c r="E111" s="54" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="F111" s="47"/>
       <c r="G111" s="45" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="H111" s="45" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="I111" s="33"/>
     </row>
@@ -4222,14 +4225,14 @@
       <c r="C112" s="32"/>
       <c r="D112" s="45"/>
       <c r="E112" s="45" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="F112" s="47"/>
       <c r="G112" s="45" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="H112" s="45" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="I112" s="33"/>
     </row>
@@ -4239,14 +4242,14 @@
       <c r="C113" s="32"/>
       <c r="D113" s="45"/>
       <c r="E113" s="54" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="F113" s="47"/>
       <c r="G113" s="45" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="H113" s="45" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="I113" s="33"/>
     </row>

</xml_diff>

<commit_message>
I added some code
</commit_message>
<xml_diff>
--- a/source_file/jquery_testscenario.xlsx
+++ b/source_file/jquery_testscenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gturd\IdeaProjects\FirstAssignment\source_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0FE29F-D286-446E-8BF0-6072760D97A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA073ED-4E10-43ED-885D-A8F0D447321C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{CE714CED-6ED2-47BF-9249-83F3ACACC2F2}"/>
   </bookViews>
@@ -2170,7 +2170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E61229-28C4-4005-AC6C-FBD77E5B6143}">
   <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
I added some code and updated source file
</commit_message>
<xml_diff>
--- a/source_file/jquery_testscenario.xlsx
+++ b/source_file/jquery_testscenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gturd\IdeaProjects\FirstAssignment\source_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA073ED-4E10-43ED-885D-A8F0D447321C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A509CA36-E142-4DD3-A166-A5491B661273}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{CE714CED-6ED2-47BF-9249-83F3ACACC2F2}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="336">
   <si>
     <t>Project Name:</t>
   </si>
@@ -1025,6 +1025,15 @@
   </si>
   <si>
     <t>The user should be able to open the browser and should be able to show additional information on context field on the Tooltip page</t>
+  </si>
+  <si>
+    <t>Verify 'Basic dialog' is resized</t>
+  </si>
+  <si>
+    <t>Basic dialog' frame should be resized</t>
+  </si>
+  <si>
+    <t>Basic dialog' frame is resized</t>
   </si>
 </sst>
 </file>
@@ -2168,10 +2177,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E61229-28C4-4005-AC6C-FBD77E5B6143}">
-  <dimension ref="A1:I115"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3610,79 +3619,79 @@
       </c>
       <c r="I78" s="33"/>
     </row>
-    <row r="79" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A79" s="30"/>
       <c r="B79" s="31"/>
       <c r="C79" s="32"/>
       <c r="D79" s="32"/>
-      <c r="E79" s="45" t="s">
+      <c r="E79" s="54" t="s">
+        <v>333</v>
+      </c>
+      <c r="F79" s="32"/>
+      <c r="G79" s="56" t="s">
+        <v>334</v>
+      </c>
+      <c r="H79" s="56" t="s">
+        <v>335</v>
+      </c>
+      <c r="I79" s="33"/>
+    </row>
+    <row r="80" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="30"/>
+      <c r="B80" s="31"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="32"/>
+      <c r="E80" s="45" t="s">
         <v>222</v>
       </c>
-      <c r="F79" s="32"/>
-      <c r="G79" s="45" t="s">
+      <c r="F80" s="32"/>
+      <c r="G80" s="45" t="s">
         <v>223</v>
       </c>
-      <c r="H79" s="45" t="s">
+      <c r="H80" s="45" t="s">
         <v>224</v>
       </c>
-      <c r="I79" s="33"/>
-    </row>
-    <row r="80" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="58" t="s">
+      <c r="I80" s="33"/>
+    </row>
+    <row r="81" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="B80" s="51" t="s">
+      <c r="B81" s="51" t="s">
         <v>225</v>
       </c>
-      <c r="C80" s="32"/>
-      <c r="D80" s="45" t="s">
+      <c r="C81" s="32"/>
+      <c r="D81" s="45" t="s">
         <v>327</v>
       </c>
-      <c r="E80" s="45" t="s">
+      <c r="E81" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="F80" s="47" t="s">
+      <c r="F81" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="G80" s="45" t="s">
+      <c r="G81" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="H80" s="45" t="s">
+      <c r="H81" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="I80" s="33"/>
-    </row>
-    <row r="81" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="30"/>
-      <c r="B81" s="31"/>
-      <c r="C81" s="32"/>
-      <c r="D81" s="32"/>
-      <c r="E81" s="45" t="s">
-        <v>226</v>
-      </c>
-      <c r="F81" s="32"/>
-      <c r="G81" s="45" t="s">
-        <v>227</v>
-      </c>
-      <c r="H81" s="45" t="s">
-        <v>228</v>
-      </c>
       <c r="I81" s="33"/>
     </row>
-    <row r="82" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A82" s="30"/>
       <c r="B82" s="31"/>
       <c r="C82" s="32"/>
       <c r="D82" s="32"/>
-      <c r="E82" s="54" t="s">
-        <v>229</v>
+      <c r="E82" s="45" t="s">
+        <v>226</v>
       </c>
       <c r="F82" s="32"/>
       <c r="G82" s="45" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H82" s="45" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I82" s="33"/>
     </row>
@@ -3691,15 +3700,15 @@
       <c r="B83" s="31"/>
       <c r="C83" s="32"/>
       <c r="D83" s="32"/>
-      <c r="E83" s="45" t="s">
-        <v>232</v>
+      <c r="E83" s="54" t="s">
+        <v>229</v>
       </c>
       <c r="F83" s="32"/>
       <c r="G83" s="45" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H83" s="45" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="I83" s="33"/>
     </row>
@@ -3708,8 +3717,8 @@
       <c r="B84" s="31"/>
       <c r="C84" s="32"/>
       <c r="D84" s="32"/>
-      <c r="E84" s="54" t="s">
-        <v>235</v>
+      <c r="E84" s="45" t="s">
+        <v>232</v>
       </c>
       <c r="F84" s="32"/>
       <c r="G84" s="45" t="s">
@@ -3720,79 +3729,79 @@
       </c>
       <c r="I84" s="33"/>
     </row>
-    <row r="85" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="58" t="s">
+    <row r="85" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A85" s="30"/>
+      <c r="B85" s="31"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="32"/>
+      <c r="E85" s="54" t="s">
+        <v>235</v>
+      </c>
+      <c r="F85" s="32"/>
+      <c r="G85" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="H85" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="I85" s="33"/>
+    </row>
+    <row r="86" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B85" s="51" t="s">
+      <c r="B86" s="51" t="s">
         <v>236</v>
       </c>
-      <c r="C85" s="32"/>
-      <c r="D85" s="45" t="s">
+      <c r="C86" s="32"/>
+      <c r="D86" s="45" t="s">
         <v>328</v>
       </c>
-      <c r="E85" s="32" t="s">
+      <c r="E86" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F85" s="47" t="s">
+      <c r="F86" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="G85" s="45" t="s">
+      <c r="G86" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="H85" s="45" t="s">
+      <c r="H86" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="I85" s="33"/>
-    </row>
-    <row r="86" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="30"/>
-      <c r="B86" s="31"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="32"/>
-      <c r="E86" s="32" t="s">
-        <v>237</v>
-      </c>
-      <c r="F86" s="32"/>
-      <c r="G86" s="45" t="s">
-        <v>238</v>
-      </c>
-      <c r="H86" s="45" t="s">
-        <v>239</v>
-      </c>
       <c r="I86" s="33"/>
     </row>
-    <row r="87" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A87" s="30"/>
       <c r="B87" s="31"/>
       <c r="C87" s="32"/>
       <c r="D87" s="32"/>
-      <c r="E87" s="54" t="s">
-        <v>240</v>
+      <c r="E87" s="32" t="s">
+        <v>237</v>
       </c>
       <c r="F87" s="32"/>
       <c r="G87" s="45" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H87" s="45" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="I87" s="33"/>
     </row>
-    <row r="88" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A88" s="30"/>
       <c r="B88" s="31"/>
       <c r="C88" s="32"/>
       <c r="D88" s="32"/>
-      <c r="E88" s="45" t="s">
-        <v>243</v>
+      <c r="E88" s="54" t="s">
+        <v>240</v>
       </c>
       <c r="F88" s="32"/>
       <c r="G88" s="45" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H88" s="45" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="I88" s="33"/>
     </row>
@@ -3802,7 +3811,7 @@
       <c r="C89" s="32"/>
       <c r="D89" s="32"/>
       <c r="E89" s="45" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="F89" s="32"/>
       <c r="G89" s="45" t="s">
@@ -3819,14 +3828,14 @@
       <c r="C90" s="32"/>
       <c r="D90" s="32"/>
       <c r="E90" s="45" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="F90" s="32"/>
       <c r="G90" s="45" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H90" s="45" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="I90" s="33"/>
     </row>
@@ -3836,7 +3845,7 @@
       <c r="C91" s="32"/>
       <c r="D91" s="32"/>
       <c r="E91" s="45" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="F91" s="32"/>
       <c r="G91" s="45" t="s">
@@ -3853,14 +3862,14 @@
       <c r="C92" s="32"/>
       <c r="D92" s="32"/>
       <c r="E92" s="45" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="F92" s="32"/>
       <c r="G92" s="45" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H92" s="45" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="I92" s="33"/>
     </row>
@@ -3870,7 +3879,7 @@
       <c r="C93" s="32"/>
       <c r="D93" s="32"/>
       <c r="E93" s="45" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="F93" s="32"/>
       <c r="G93" s="45" t="s">
@@ -3887,14 +3896,14 @@
       <c r="C94" s="32"/>
       <c r="D94" s="32"/>
       <c r="E94" s="45" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="F94" s="32"/>
       <c r="G94" s="45" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H94" s="45" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="I94" s="33"/>
     </row>
@@ -3903,8 +3912,8 @@
       <c r="B95" s="31"/>
       <c r="C95" s="32"/>
       <c r="D95" s="32"/>
-      <c r="E95" s="53" t="s">
-        <v>258</v>
+      <c r="E95" s="45" t="s">
+        <v>252</v>
       </c>
       <c r="F95" s="32"/>
       <c r="G95" s="45" t="s">
@@ -3915,62 +3924,62 @@
       </c>
       <c r="I95" s="33"/>
     </row>
-    <row r="96" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A96" s="58" t="s">
+    <row r="96" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="30"/>
+      <c r="B96" s="31"/>
+      <c r="C96" s="32"/>
+      <c r="D96" s="32"/>
+      <c r="E96" s="53" t="s">
+        <v>258</v>
+      </c>
+      <c r="F96" s="32"/>
+      <c r="G96" s="45" t="s">
+        <v>253</v>
+      </c>
+      <c r="H96" s="45" t="s">
+        <v>254</v>
+      </c>
+      <c r="I96" s="33"/>
+    </row>
+    <row r="97" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A97" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="B96" s="51" t="s">
+      <c r="B97" s="51" t="s">
         <v>259</v>
       </c>
-      <c r="C96" s="32"/>
-      <c r="D96" s="45" t="s">
+      <c r="C97" s="32"/>
+      <c r="D97" s="45" t="s">
         <v>329</v>
       </c>
-      <c r="E96" s="32" t="s">
+      <c r="E97" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F96" s="47" t="s">
+      <c r="F97" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="G96" s="45" t="s">
+      <c r="G97" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="H96" s="45" t="s">
+      <c r="H97" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="I96" s="33"/>
-    </row>
-    <row r="97" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="30"/>
-      <c r="B97" s="31"/>
-      <c r="C97" s="32"/>
-      <c r="D97" s="32"/>
-      <c r="E97" s="32" t="s">
-        <v>260</v>
-      </c>
-      <c r="F97" s="32"/>
-      <c r="G97" s="45" t="s">
-        <v>261</v>
-      </c>
-      <c r="H97" s="45" t="s">
-        <v>262</v>
-      </c>
       <c r="I97" s="33"/>
     </row>
-    <row r="98" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A98" s="30"/>
       <c r="B98" s="31"/>
       <c r="C98" s="32"/>
       <c r="D98" s="32"/>
-      <c r="E98" s="54" t="s">
-        <v>263</v>
+      <c r="E98" s="32" t="s">
+        <v>260</v>
       </c>
       <c r="F98" s="32"/>
       <c r="G98" s="45" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H98" s="45" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="I98" s="33"/>
     </row>
@@ -3979,15 +3988,15 @@
       <c r="B99" s="31"/>
       <c r="C99" s="32"/>
       <c r="D99" s="32"/>
-      <c r="E99" s="45" t="s">
-        <v>266</v>
+      <c r="E99" s="54" t="s">
+        <v>263</v>
       </c>
       <c r="F99" s="32"/>
       <c r="G99" s="45" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H99" s="45" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="I99" s="33"/>
     </row>
@@ -3996,8 +4005,8 @@
       <c r="B100" s="31"/>
       <c r="C100" s="32"/>
       <c r="D100" s="32"/>
-      <c r="E100" s="54" t="s">
-        <v>269</v>
+      <c r="E100" s="45" t="s">
+        <v>266</v>
       </c>
       <c r="F100" s="32"/>
       <c r="G100" s="45" t="s">
@@ -4008,62 +4017,62 @@
       </c>
       <c r="I100" s="33"/>
     </row>
-    <row r="101" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="58" t="s">
+    <row r="101" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A101" s="30"/>
+      <c r="B101" s="31"/>
+      <c r="C101" s="32"/>
+      <c r="D101" s="32"/>
+      <c r="E101" s="54" t="s">
+        <v>269</v>
+      </c>
+      <c r="F101" s="32"/>
+      <c r="G101" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="H101" s="45" t="s">
+        <v>268</v>
+      </c>
+      <c r="I101" s="33"/>
+    </row>
+    <row r="102" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="B101" s="51" t="s">
+      <c r="B102" s="51" t="s">
         <v>270</v>
       </c>
-      <c r="C101" s="32"/>
-      <c r="D101" s="45" t="s">
+      <c r="C102" s="32"/>
+      <c r="D102" s="45" t="s">
         <v>330</v>
       </c>
-      <c r="E101" s="45" t="s">
+      <c r="E102" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="F101" s="47" t="s">
+      <c r="F102" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="G101" s="45" t="s">
+      <c r="G102" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="H101" s="45" t="s">
+      <c r="H102" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="I101" s="33"/>
-    </row>
-    <row r="102" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="30"/>
-      <c r="B102" s="31"/>
-      <c r="C102" s="32"/>
-      <c r="D102" s="32"/>
-      <c r="E102" s="45" t="s">
-        <v>271</v>
-      </c>
-      <c r="F102" s="32"/>
-      <c r="G102" s="45" t="s">
-        <v>272</v>
-      </c>
-      <c r="H102" s="45" t="s">
-        <v>273</v>
-      </c>
       <c r="I102" s="33"/>
     </row>
-    <row r="103" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A103" s="30"/>
       <c r="B103" s="31"/>
       <c r="C103" s="32"/>
       <c r="D103" s="32"/>
       <c r="E103" s="45" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F103" s="32"/>
       <c r="G103" s="45" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="H103" s="45" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="I103" s="33"/>
     </row>
@@ -4072,177 +4081,177 @@
       <c r="B104" s="31"/>
       <c r="C104" s="32"/>
       <c r="D104" s="32"/>
-      <c r="E104" s="54" t="s">
-        <v>279</v>
+      <c r="E104" s="45" t="s">
+        <v>274</v>
       </c>
       <c r="F104" s="32"/>
       <c r="G104" s="45" t="s">
+        <v>275</v>
+      </c>
+      <c r="H104" s="45" t="s">
+        <v>276</v>
+      </c>
+      <c r="I104" s="33"/>
+    </row>
+    <row r="105" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="A105" s="30"/>
+      <c r="B105" s="31"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="32"/>
+      <c r="E105" s="54" t="s">
+        <v>279</v>
+      </c>
+      <c r="F105" s="32"/>
+      <c r="G105" s="45" t="s">
         <v>278</v>
       </c>
-      <c r="H104" s="45" t="s">
+      <c r="H105" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="I104" s="33"/>
-    </row>
-    <row r="105" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A105" s="58" t="s">
+      <c r="I105" s="33"/>
+    </row>
+    <row r="106" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A106" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="B105" s="51" t="s">
+      <c r="B106" s="51" t="s">
         <v>280</v>
       </c>
-      <c r="C105" s="32"/>
-      <c r="D105" s="45" t="s">
+      <c r="C106" s="32"/>
+      <c r="D106" s="45" t="s">
         <v>331</v>
       </c>
-      <c r="E105" s="45" t="s">
+      <c r="E106" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="F105" s="47" t="s">
+      <c r="F106" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="G105" s="45" t="s">
+      <c r="G106" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="H105" s="45" t="s">
+      <c r="H106" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="I105" s="33"/>
-    </row>
-    <row r="106" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="A106" s="30"/>
-      <c r="B106" s="31"/>
-      <c r="C106" s="32"/>
-      <c r="D106" s="32"/>
-      <c r="E106" s="45" t="s">
-        <v>281</v>
-      </c>
-      <c r="F106" s="32"/>
-      <c r="G106" s="45" t="s">
-        <v>282</v>
-      </c>
-      <c r="H106" s="45" t="s">
-        <v>283</v>
-      </c>
       <c r="I106" s="33"/>
     </row>
-    <row r="107" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A107" s="30"/>
       <c r="B107" s="31"/>
       <c r="C107" s="32"/>
       <c r="D107" s="32"/>
-      <c r="E107" s="60" t="s">
-        <v>285</v>
+      <c r="E107" s="45" t="s">
+        <v>281</v>
       </c>
       <c r="F107" s="32"/>
       <c r="G107" s="45" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="H107" s="45" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="I107" s="33"/>
     </row>
-    <row r="108" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A108" s="30"/>
       <c r="B108" s="31"/>
       <c r="C108" s="32"/>
       <c r="D108" s="32"/>
-      <c r="E108" s="59" t="s">
-        <v>284</v>
+      <c r="E108" s="60" t="s">
+        <v>285</v>
       </c>
       <c r="F108" s="32"/>
       <c r="G108" s="45" t="s">
+        <v>286</v>
+      </c>
+      <c r="H108" s="45" t="s">
+        <v>287</v>
+      </c>
+      <c r="I108" s="33"/>
+    </row>
+    <row r="109" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A109" s="30"/>
+      <c r="B109" s="31"/>
+      <c r="C109" s="32"/>
+      <c r="D109" s="32"/>
+      <c r="E109" s="59" t="s">
+        <v>284</v>
+      </c>
+      <c r="F109" s="32"/>
+      <c r="G109" s="45" t="s">
         <v>288</v>
       </c>
-      <c r="H108" s="45" t="s">
+      <c r="H109" s="45" t="s">
         <v>289</v>
       </c>
-      <c r="I108" s="33"/>
-    </row>
-    <row r="109" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A109" s="58" t="s">
+      <c r="I109" s="33"/>
+    </row>
+    <row r="110" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A110" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B109" s="51" t="s">
+      <c r="B110" s="51" t="s">
         <v>290</v>
       </c>
-      <c r="C109" s="32"/>
-      <c r="D109" s="45" t="s">
+      <c r="C110" s="32"/>
+      <c r="D110" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="E109" s="45" t="s">
+      <c r="E110" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="F109" s="47" t="s">
+      <c r="F110" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="G109" s="45" t="s">
+      <c r="G110" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="H109" s="45" t="s">
+      <c r="H110" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="I109" s="33"/>
-    </row>
-    <row r="110" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="58"/>
-      <c r="B110" s="51"/>
-      <c r="C110" s="32"/>
-      <c r="D110" s="45"/>
-      <c r="E110" s="45" t="s">
-        <v>291</v>
-      </c>
-      <c r="F110" s="47"/>
-      <c r="G110" s="45" t="s">
-        <v>292</v>
-      </c>
-      <c r="H110" s="45" t="s">
-        <v>293</v>
-      </c>
       <c r="I110" s="33"/>
     </row>
-    <row r="111" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A111" s="58"/>
       <c r="B111" s="51"/>
       <c r="C111" s="32"/>
       <c r="D111" s="45"/>
-      <c r="E111" s="54" t="s">
-        <v>295</v>
+      <c r="E111" s="45" t="s">
+        <v>291</v>
       </c>
       <c r="F111" s="47"/>
       <c r="G111" s="45" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="H111" s="45" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="I111" s="33"/>
     </row>
-    <row r="112" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A112" s="58"/>
       <c r="B112" s="51"/>
       <c r="C112" s="32"/>
       <c r="D112" s="45"/>
-      <c r="E112" s="45" t="s">
-        <v>300</v>
+      <c r="E112" s="54" t="s">
+        <v>295</v>
       </c>
       <c r="F112" s="47"/>
       <c r="G112" s="45" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H112" s="45" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I112" s="33"/>
     </row>
-    <row r="113" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A113" s="58"/>
       <c r="B113" s="51"/>
       <c r="C113" s="32"/>
       <c r="D113" s="45"/>
-      <c r="E113" s="54" t="s">
-        <v>299</v>
+      <c r="E113" s="45" t="s">
+        <v>300</v>
       </c>
       <c r="F113" s="47"/>
       <c r="G113" s="45" t="s">
@@ -4253,27 +4262,44 @@
       </c>
       <c r="I113" s="33"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="30"/>
-      <c r="B114" s="31"/>
+    <row r="114" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A114" s="58"/>
+      <c r="B114" s="51"/>
       <c r="C114" s="32"/>
-      <c r="D114" s="32"/>
-      <c r="E114" s="32"/>
-      <c r="F114" s="32"/>
-      <c r="G114" s="32"/>
-      <c r="H114" s="32"/>
+      <c r="D114" s="45"/>
+      <c r="E114" s="54" t="s">
+        <v>299</v>
+      </c>
+      <c r="F114" s="47"/>
+      <c r="G114" s="45" t="s">
+        <v>294</v>
+      </c>
+      <c r="H114" s="45" t="s">
+        <v>298</v>
+      </c>
       <c r="I114" s="33"/>
     </row>
-    <row r="115" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="34"/>
-      <c r="B115" s="35"/>
-      <c r="C115" s="36"/>
-      <c r="D115" s="36"/>
-      <c r="E115" s="36"/>
-      <c r="F115" s="36"/>
-      <c r="G115" s="36"/>
-      <c r="H115" s="36"/>
-      <c r="I115" s="37"/>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="30"/>
+      <c r="B115" s="31"/>
+      <c r="C115" s="32"/>
+      <c r="D115" s="32"/>
+      <c r="E115" s="32"/>
+      <c r="F115" s="32"/>
+      <c r="G115" s="32"/>
+      <c r="H115" s="32"/>
+      <c r="I115" s="33"/>
+    </row>
+    <row r="116" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="34"/>
+      <c r="B116" s="35"/>
+      <c r="C116" s="36"/>
+      <c r="D116" s="36"/>
+      <c r="E116" s="36"/>
+      <c r="F116" s="36"/>
+      <c r="G116" s="36"/>
+      <c r="H116" s="36"/>
+      <c r="I116" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4294,12 +4320,12 @@
     <hyperlink ref="F63" r:id="rId10" xr:uid="{38C773A1-3BC7-4C3B-86E6-BF32F3AD4C6E}"/>
     <hyperlink ref="F68" r:id="rId11" xr:uid="{7F4F6A8C-AA17-4340-A40E-12303FEF29BC}"/>
     <hyperlink ref="F75" r:id="rId12" xr:uid="{628B29C5-A280-4C65-B16F-9229BD446432}"/>
-    <hyperlink ref="F80" r:id="rId13" xr:uid="{0F214E2E-2D9B-48C2-AA50-AA0E7B1CD847}"/>
-    <hyperlink ref="F85" r:id="rId14" xr:uid="{018D8B70-E240-478A-877C-1B64E2B66707}"/>
-    <hyperlink ref="F96" r:id="rId15" xr:uid="{33E612D4-2082-4338-AAF2-0EE5AFFF32D1}"/>
-    <hyperlink ref="F101" r:id="rId16" xr:uid="{B72CDD78-A935-497F-9CB9-CA194A8DA39D}"/>
-    <hyperlink ref="F105" r:id="rId17" xr:uid="{757F55F1-53F2-4ABC-9889-CDDE44904BFB}"/>
-    <hyperlink ref="F109" r:id="rId18" xr:uid="{1033D818-4443-48C9-B429-21937673AF2E}"/>
+    <hyperlink ref="F81" r:id="rId13" xr:uid="{0F214E2E-2D9B-48C2-AA50-AA0E7B1CD847}"/>
+    <hyperlink ref="F86" r:id="rId14" xr:uid="{018D8B70-E240-478A-877C-1B64E2B66707}"/>
+    <hyperlink ref="F97" r:id="rId15" xr:uid="{33E612D4-2082-4338-AAF2-0EE5AFFF32D1}"/>
+    <hyperlink ref="F102" r:id="rId16" xr:uid="{B72CDD78-A935-497F-9CB9-CA194A8DA39D}"/>
+    <hyperlink ref="F106" r:id="rId17" xr:uid="{757F55F1-53F2-4ABC-9889-CDDE44904BFB}"/>
+    <hyperlink ref="F110" r:id="rId18" xr:uid="{1033D818-4443-48C9-B429-21937673AF2E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>

</xml_diff>

<commit_message>
I added some code and also added some data to the source file
</commit_message>
<xml_diff>
--- a/source_file/jquery_testscenario.xlsx
+++ b/source_file/jquery_testscenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gturd\IdeaProjects\FirstAssignment\source_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A509CA36-E142-4DD3-A166-A5491B661273}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29911BDC-E03C-4C0C-951F-6819FBF82792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{CE714CED-6ED2-47BF-9249-83F3ACACC2F2}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="348">
   <si>
     <t>Project Name:</t>
   </si>
@@ -1034,6 +1034,42 @@
   </si>
   <si>
     <t>Basic dialog' frame is resized</t>
+  </si>
+  <si>
+    <t>Faster</t>
+  </si>
+  <si>
+    <t>ui.jQuery.js</t>
+  </si>
+  <si>
+    <t>Dr.</t>
+  </si>
+  <si>
+    <t>XOffset = 100            Yoffset = 100</t>
+  </si>
+  <si>
+    <t>XOffset = 200            Yoffset = 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    5 Star</t>
+  </si>
+  <si>
+    <t>Automatic, Insurance, 1</t>
+  </si>
+  <si>
+    <t>May/28/2021</t>
+  </si>
+  <si>
+    <t>Xoffset = 400, Yoffset = 50</t>
+  </si>
+  <si>
+    <t>Music, Pop</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1629,6 +1665,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2179,8 +2218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E61229-28C4-4005-AC6C-FBD77E5B6143}">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H79" sqref="H79"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2422,7 +2461,9 @@
       <c r="E14" s="45" t="s">
         <v>312</v>
       </c>
-      <c r="F14" s="32"/>
+      <c r="F14" s="45" t="s">
+        <v>339</v>
+      </c>
       <c r="G14" s="45" t="s">
         <v>313</v>
       </c>
@@ -2612,7 +2653,9 @@
       <c r="E24" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="F24" s="32"/>
+      <c r="F24" s="45" t="s">
+        <v>340</v>
+      </c>
       <c r="G24" s="45" t="s">
         <v>96</v>
       </c>
@@ -3043,7 +3086,9 @@
       <c r="E47" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="F47" s="32"/>
+      <c r="F47" s="66" t="s">
+        <v>341</v>
+      </c>
       <c r="G47" s="45" t="s">
         <v>149</v>
       </c>
@@ -3263,7 +3308,9 @@
       <c r="E59" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="F59" s="32"/>
+      <c r="F59" s="32" t="s">
+        <v>342</v>
+      </c>
       <c r="G59" s="56" t="s">
         <v>175</v>
       </c>
@@ -3297,7 +3344,9 @@
       <c r="E61" s="45" t="s">
         <v>179</v>
       </c>
-      <c r="F61" s="32"/>
+      <c r="F61" s="32" t="s">
+        <v>343</v>
+      </c>
       <c r="G61" s="45" t="s">
         <v>180</v>
       </c>
@@ -3390,7 +3439,9 @@
       <c r="E66" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="F66" s="32"/>
+      <c r="F66" s="45" t="s">
+        <v>344</v>
+      </c>
       <c r="G66" s="45" t="s">
         <v>191</v>
       </c>
@@ -3483,7 +3534,9 @@
       <c r="E71" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="F71" s="32"/>
+      <c r="F71" s="32" t="s">
+        <v>345</v>
+      </c>
       <c r="G71" s="45" t="s">
         <v>203</v>
       </c>
@@ -3497,7 +3550,7 @@
       <c r="B72" s="31"/>
       <c r="C72" s="32"/>
       <c r="D72" s="32"/>
-      <c r="E72" s="45" t="s">
+      <c r="E72" s="54" t="s">
         <v>205</v>
       </c>
       <c r="F72" s="32"/>
@@ -3610,7 +3663,9 @@
       <c r="E78" s="45" t="s">
         <v>220</v>
       </c>
-      <c r="F78" s="32"/>
+      <c r="F78" s="45" t="s">
+        <v>346</v>
+      </c>
       <c r="G78" s="45" t="s">
         <v>219</v>
       </c>
@@ -3720,7 +3775,9 @@
       <c r="E84" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="F84" s="32"/>
+      <c r="F84" s="32" t="s">
+        <v>347</v>
+      </c>
       <c r="G84" s="45" t="s">
         <v>233</v>
       </c>
@@ -3813,7 +3870,9 @@
       <c r="E89" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="F89" s="32"/>
+      <c r="F89" s="32" t="s">
+        <v>336</v>
+      </c>
       <c r="G89" s="45" t="s">
         <v>244</v>
       </c>
@@ -3827,7 +3886,7 @@
       <c r="B90" s="31"/>
       <c r="C90" s="32"/>
       <c r="D90" s="32"/>
-      <c r="E90" s="45" t="s">
+      <c r="E90" s="54" t="s">
         <v>255</v>
       </c>
       <c r="F90" s="32"/>
@@ -3847,7 +3906,9 @@
       <c r="E91" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="F91" s="32"/>
+      <c r="F91" s="32" t="s">
+        <v>337</v>
+      </c>
       <c r="G91" s="45" t="s">
         <v>247</v>
       </c>
@@ -3861,7 +3922,7 @@
       <c r="B92" s="31"/>
       <c r="C92" s="32"/>
       <c r="D92" s="32"/>
-      <c r="E92" s="45" t="s">
+      <c r="E92" s="54" t="s">
         <v>256</v>
       </c>
       <c r="F92" s="32"/>
@@ -3881,7 +3942,9 @@
       <c r="E93" s="45" t="s">
         <v>249</v>
       </c>
-      <c r="F93" s="32"/>
+      <c r="F93" s="32">
+        <v>3</v>
+      </c>
       <c r="G93" s="45" t="s">
         <v>250</v>
       </c>
@@ -3895,7 +3958,7 @@
       <c r="B94" s="31"/>
       <c r="C94" s="32"/>
       <c r="D94" s="32"/>
-      <c r="E94" s="45" t="s">
+      <c r="E94" s="54" t="s">
         <v>257</v>
       </c>
       <c r="F94" s="32"/>
@@ -3915,7 +3978,9 @@
       <c r="E95" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="F95" s="32"/>
+      <c r="F95" s="32" t="s">
+        <v>338</v>
+      </c>
       <c r="G95" s="45" t="s">
         <v>253</v>
       </c>
@@ -4008,7 +4073,9 @@
       <c r="E100" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="F100" s="32"/>
+      <c r="F100" s="32">
+        <v>400</v>
+      </c>
       <c r="G100" s="45" t="s">
         <v>267</v>
       </c>
@@ -4084,7 +4151,9 @@
       <c r="E104" s="45" t="s">
         <v>274</v>
       </c>
-      <c r="F104" s="32"/>
+      <c r="F104" s="32">
+        <v>12</v>
+      </c>
       <c r="G104" s="45" t="s">
         <v>275</v>
       </c>
@@ -4253,7 +4322,9 @@
       <c r="E113" s="45" t="s">
         <v>300</v>
       </c>
-      <c r="F113" s="47"/>
+      <c r="F113" s="47">
+        <v>45</v>
+      </c>
       <c r="G113" s="45" t="s">
         <v>294</v>
       </c>

</xml_diff>

<commit_message>
I added priority to the @Test
</commit_message>
<xml_diff>
--- a/source_file/jquery_testscenario.xlsx
+++ b/source_file/jquery_testscenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gturd\IdeaProjects\FirstAssignment\source_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29911BDC-E03C-4C0C-951F-6819FBF82792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8740E7F3-443E-4785-ACF8-EEDD19DDF695}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{CE714CED-6ED2-47BF-9249-83F3ACACC2F2}"/>
   </bookViews>
@@ -1651,6 +1651,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1665,9 +1668,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2218,7 +2218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E61229-28C4-4005-AC6C-FBD77E5B6143}">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
@@ -2235,7 +2235,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2256,7 +2256,7 @@
       <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="62"/>
+      <c r="A2" s="63"/>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
@@ -2317,26 +2317,26 @@
       <c r="A6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
       <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3086,7 +3086,7 @@
       <c r="E47" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="F47" s="66" t="s">
+      <c r="F47" s="61" t="s">
         <v>341</v>
       </c>
       <c r="G47" s="45" t="s">

</xml_diff>

<commit_message>
I have written test scenarios, test cases and test steps on the excel spreadsheet and based on the test steps I have written code using java with selenium webdriver.
</commit_message>
<xml_diff>
--- a/source_file/jquery_testscenario.xlsx
+++ b/source_file/jquery_testscenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gturd\IdeaProjects\FirstAssignment\source_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8740E7F3-443E-4785-ACF8-EEDD19DDF695}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC314C9B-1608-4F43-8B21-C91E909D04A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{CE714CED-6ED2-47BF-9249-83F3ACACC2F2}"/>
   </bookViews>
@@ -2218,8 +2218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E61229-28C4-4005-AC6C-FBD77E5B6143}">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>